<commit_message>
Fixing the button on the Declaration in V11bi (and tweaking the localisation tags).
</commit_message>
<xml_diff>
--- a/app/data/MCCD-localisation-V01.xlsx
+++ b/app/data/MCCD-localisation-V01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JALAT/GIT/medical-certificate-of-cause-of-death/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055A3F6B-5713-944D-9832-6C33EF35B4C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC288FEB-3F7A-1A4F-8D3B-7D120D1DDD8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13940" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13940" firstSheet="3" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Using this document" sheetId="8" r:id="rId1"/>
@@ -3024,9 +3024,6 @@
     <t>AP Declaration content.</t>
   </si>
   <si>
-    <t>apDeclarationSubmitForScrutiny</t>
-  </si>
-  <si>
     <t>meScrutinyDeclarationPageTitle</t>
   </si>
   <si>
@@ -3036,9 +3033,6 @@
     <t>meScrutinyDeclarationContent</t>
   </si>
   <si>
-    <t>meScrutinyReadyForRegistrar</t>
-  </si>
-  <si>
     <t>meCertDeclarationPageTitle</t>
   </si>
   <si>
@@ -3058,9 +3052,6 @@
   </si>
   <si>
     <t>MEO Declaration content.</t>
-  </si>
-  <si>
-    <t>meoDeclarationSubmitForScrutiny</t>
   </si>
   <si>
     <t>confirmationPageTitle</t>
@@ -4469,6 +4460,15 @@
       </rPr>
       <t>.</t>
     </r>
+  </si>
+  <si>
+    <t>apDeclarationSubmitForScrutinyCTA</t>
+  </si>
+  <si>
+    <t>meScrutinyReadyForRegisterOfficeCTA</t>
+  </si>
+  <si>
+    <t>meoDeclarationSubmitForScrutinyCTA</t>
   </si>
 </sst>
 </file>
@@ -4969,7 +4969,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="215">
+  <cellXfs count="214">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -5484,6 +5484,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -5496,6 +5499,24 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -5505,24 +5526,6 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -5594,12 +5597,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5623,10 +5620,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5935,538 +5928,538 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="176" t="s">
+      <c r="A1" s="177" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="176"/>
-      <c r="C1" s="176"/>
-      <c r="D1" s="176"/>
-      <c r="E1" s="176"/>
-      <c r="F1" s="176"/>
-      <c r="G1" s="176"/>
-      <c r="H1" s="176"/>
-      <c r="I1" s="176"/>
-      <c r="J1" s="176"/>
-      <c r="K1" s="176"/>
-      <c r="L1" s="176"/>
+      <c r="B1" s="177"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="177"/>
+      <c r="G1" s="177"/>
+      <c r="H1" s="177"/>
+      <c r="I1" s="177"/>
+      <c r="J1" s="177"/>
+      <c r="K1" s="177"/>
+      <c r="L1" s="177"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="176"/>
-      <c r="B2" s="176"/>
-      <c r="C2" s="176"/>
-      <c r="D2" s="176"/>
-      <c r="E2" s="176"/>
-      <c r="F2" s="176"/>
-      <c r="G2" s="176"/>
-      <c r="H2" s="176"/>
-      <c r="I2" s="176"/>
-      <c r="J2" s="176"/>
-      <c r="K2" s="176"/>
-      <c r="L2" s="176"/>
+      <c r="A2" s="177"/>
+      <c r="B2" s="177"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177"/>
+      <c r="H2" s="177"/>
+      <c r="I2" s="177"/>
+      <c r="J2" s="177"/>
+      <c r="K2" s="177"/>
+      <c r="L2" s="177"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="176"/>
-      <c r="B3" s="176"/>
-      <c r="C3" s="176"/>
-      <c r="D3" s="176"/>
-      <c r="E3" s="176"/>
-      <c r="F3" s="176"/>
-      <c r="G3" s="176"/>
-      <c r="H3" s="176"/>
-      <c r="I3" s="176"/>
-      <c r="J3" s="176"/>
-      <c r="K3" s="176"/>
-      <c r="L3" s="176"/>
+      <c r="A3" s="177"/>
+      <c r="B3" s="177"/>
+      <c r="C3" s="177"/>
+      <c r="D3" s="177"/>
+      <c r="E3" s="177"/>
+      <c r="F3" s="177"/>
+      <c r="G3" s="177"/>
+      <c r="H3" s="177"/>
+      <c r="I3" s="177"/>
+      <c r="J3" s="177"/>
+      <c r="K3" s="177"/>
+      <c r="L3" s="177"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="176"/>
-      <c r="B4" s="176"/>
-      <c r="C4" s="176"/>
-      <c r="D4" s="176"/>
-      <c r="E4" s="176"/>
-      <c r="F4" s="176"/>
-      <c r="G4" s="176"/>
-      <c r="H4" s="176"/>
-      <c r="I4" s="176"/>
-      <c r="J4" s="176"/>
-      <c r="K4" s="176"/>
-      <c r="L4" s="176"/>
+      <c r="A4" s="177"/>
+      <c r="B4" s="177"/>
+      <c r="C4" s="177"/>
+      <c r="D4" s="177"/>
+      <c r="E4" s="177"/>
+      <c r="F4" s="177"/>
+      <c r="G4" s="177"/>
+      <c r="H4" s="177"/>
+      <c r="I4" s="177"/>
+      <c r="J4" s="177"/>
+      <c r="K4" s="177"/>
+      <c r="L4" s="177"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="176"/>
-      <c r="B5" s="176"/>
-      <c r="C5" s="176"/>
-      <c r="D5" s="176"/>
-      <c r="E5" s="176"/>
-      <c r="F5" s="176"/>
-      <c r="G5" s="176"/>
-      <c r="H5" s="176"/>
-      <c r="I5" s="176"/>
-      <c r="J5" s="176"/>
-      <c r="K5" s="176"/>
-      <c r="L5" s="176"/>
+      <c r="A5" s="177"/>
+      <c r="B5" s="177"/>
+      <c r="C5" s="177"/>
+      <c r="D5" s="177"/>
+      <c r="E5" s="177"/>
+      <c r="F5" s="177"/>
+      <c r="G5" s="177"/>
+      <c r="H5" s="177"/>
+      <c r="I5" s="177"/>
+      <c r="J5" s="177"/>
+      <c r="K5" s="177"/>
+      <c r="L5" s="177"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="176"/>
-      <c r="B6" s="176"/>
-      <c r="C6" s="176"/>
-      <c r="D6" s="176"/>
-      <c r="E6" s="176"/>
-      <c r="F6" s="176"/>
-      <c r="G6" s="176"/>
-      <c r="H6" s="176"/>
-      <c r="I6" s="176"/>
-      <c r="J6" s="176"/>
-      <c r="K6" s="176"/>
-      <c r="L6" s="176"/>
+      <c r="A6" s="177"/>
+      <c r="B6" s="177"/>
+      <c r="C6" s="177"/>
+      <c r="D6" s="177"/>
+      <c r="E6" s="177"/>
+      <c r="F6" s="177"/>
+      <c r="G6" s="177"/>
+      <c r="H6" s="177"/>
+      <c r="I6" s="177"/>
+      <c r="J6" s="177"/>
+      <c r="K6" s="177"/>
+      <c r="L6" s="177"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="176"/>
-      <c r="B7" s="176"/>
-      <c r="C7" s="176"/>
-      <c r="D7" s="176"/>
-      <c r="E7" s="176"/>
-      <c r="F7" s="176"/>
-      <c r="G7" s="176"/>
-      <c r="H7" s="176"/>
-      <c r="I7" s="176"/>
-      <c r="J7" s="176"/>
-      <c r="K7" s="176"/>
-      <c r="L7" s="176"/>
+      <c r="A7" s="177"/>
+      <c r="B7" s="177"/>
+      <c r="C7" s="177"/>
+      <c r="D7" s="177"/>
+      <c r="E7" s="177"/>
+      <c r="F7" s="177"/>
+      <c r="G7" s="177"/>
+      <c r="H7" s="177"/>
+      <c r="I7" s="177"/>
+      <c r="J7" s="177"/>
+      <c r="K7" s="177"/>
+      <c r="L7" s="177"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="176"/>
-      <c r="B8" s="176"/>
-      <c r="C8" s="176"/>
-      <c r="D8" s="176"/>
-      <c r="E8" s="176"/>
-      <c r="F8" s="176"/>
-      <c r="G8" s="176"/>
-      <c r="H8" s="176"/>
-      <c r="I8" s="176"/>
-      <c r="J8" s="176"/>
-      <c r="K8" s="176"/>
-      <c r="L8" s="176"/>
+      <c r="A8" s="177"/>
+      <c r="B8" s="177"/>
+      <c r="C8" s="177"/>
+      <c r="D8" s="177"/>
+      <c r="E8" s="177"/>
+      <c r="F8" s="177"/>
+      <c r="G8" s="177"/>
+      <c r="H8" s="177"/>
+      <c r="I8" s="177"/>
+      <c r="J8" s="177"/>
+      <c r="K8" s="177"/>
+      <c r="L8" s="177"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="176"/>
-      <c r="B9" s="176"/>
-      <c r="C9" s="176"/>
-      <c r="D9" s="176"/>
-      <c r="E9" s="176"/>
-      <c r="F9" s="176"/>
-      <c r="G9" s="176"/>
-      <c r="H9" s="176"/>
-      <c r="I9" s="176"/>
-      <c r="J9" s="176"/>
-      <c r="K9" s="176"/>
-      <c r="L9" s="176"/>
+      <c r="A9" s="177"/>
+      <c r="B9" s="177"/>
+      <c r="C9" s="177"/>
+      <c r="D9" s="177"/>
+      <c r="E9" s="177"/>
+      <c r="F9" s="177"/>
+      <c r="G9" s="177"/>
+      <c r="H9" s="177"/>
+      <c r="I9" s="177"/>
+      <c r="J9" s="177"/>
+      <c r="K9" s="177"/>
+      <c r="L9" s="177"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="176"/>
-      <c r="B10" s="176"/>
-      <c r="C10" s="176"/>
-      <c r="D10" s="176"/>
-      <c r="E10" s="176"/>
-      <c r="F10" s="176"/>
-      <c r="G10" s="176"/>
-      <c r="H10" s="176"/>
-      <c r="I10" s="176"/>
-      <c r="J10" s="176"/>
-      <c r="K10" s="176"/>
-      <c r="L10" s="176"/>
+      <c r="A10" s="177"/>
+      <c r="B10" s="177"/>
+      <c r="C10" s="177"/>
+      <c r="D10" s="177"/>
+      <c r="E10" s="177"/>
+      <c r="F10" s="177"/>
+      <c r="G10" s="177"/>
+      <c r="H10" s="177"/>
+      <c r="I10" s="177"/>
+      <c r="J10" s="177"/>
+      <c r="K10" s="177"/>
+      <c r="L10" s="177"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="176"/>
-      <c r="B11" s="176"/>
-      <c r="C11" s="176"/>
-      <c r="D11" s="176"/>
-      <c r="E11" s="176"/>
-      <c r="F11" s="176"/>
-      <c r="G11" s="176"/>
-      <c r="H11" s="176"/>
-      <c r="I11" s="176"/>
-      <c r="J11" s="176"/>
-      <c r="K11" s="176"/>
-      <c r="L11" s="176"/>
+      <c r="A11" s="177"/>
+      <c r="B11" s="177"/>
+      <c r="C11" s="177"/>
+      <c r="D11" s="177"/>
+      <c r="E11" s="177"/>
+      <c r="F11" s="177"/>
+      <c r="G11" s="177"/>
+      <c r="H11" s="177"/>
+      <c r="I11" s="177"/>
+      <c r="J11" s="177"/>
+      <c r="K11" s="177"/>
+      <c r="L11" s="177"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="176"/>
-      <c r="B12" s="176"/>
-      <c r="C12" s="176"/>
-      <c r="D12" s="176"/>
-      <c r="E12" s="176"/>
-      <c r="F12" s="176"/>
-      <c r="G12" s="176"/>
-      <c r="H12" s="176"/>
-      <c r="I12" s="176"/>
-      <c r="J12" s="176"/>
-      <c r="K12" s="176"/>
-      <c r="L12" s="176"/>
+      <c r="A12" s="177"/>
+      <c r="B12" s="177"/>
+      <c r="C12" s="177"/>
+      <c r="D12" s="177"/>
+      <c r="E12" s="177"/>
+      <c r="F12" s="177"/>
+      <c r="G12" s="177"/>
+      <c r="H12" s="177"/>
+      <c r="I12" s="177"/>
+      <c r="J12" s="177"/>
+      <c r="K12" s="177"/>
+      <c r="L12" s="177"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="176"/>
-      <c r="B13" s="176"/>
-      <c r="C13" s="176"/>
-      <c r="D13" s="176"/>
-      <c r="E13" s="176"/>
-      <c r="F13" s="176"/>
-      <c r="G13" s="176"/>
-      <c r="H13" s="176"/>
-      <c r="I13" s="176"/>
-      <c r="J13" s="176"/>
-      <c r="K13" s="176"/>
-      <c r="L13" s="176"/>
+      <c r="A13" s="177"/>
+      <c r="B13" s="177"/>
+      <c r="C13" s="177"/>
+      <c r="D13" s="177"/>
+      <c r="E13" s="177"/>
+      <c r="F13" s="177"/>
+      <c r="G13" s="177"/>
+      <c r="H13" s="177"/>
+      <c r="I13" s="177"/>
+      <c r="J13" s="177"/>
+      <c r="K13" s="177"/>
+      <c r="L13" s="177"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="176"/>
-      <c r="B14" s="176"/>
-      <c r="C14" s="176"/>
-      <c r="D14" s="176"/>
-      <c r="E14" s="176"/>
-      <c r="F14" s="176"/>
-      <c r="G14" s="176"/>
-      <c r="H14" s="176"/>
-      <c r="I14" s="176"/>
-      <c r="J14" s="176"/>
-      <c r="K14" s="176"/>
-      <c r="L14" s="176"/>
+      <c r="A14" s="177"/>
+      <c r="B14" s="177"/>
+      <c r="C14" s="177"/>
+      <c r="D14" s="177"/>
+      <c r="E14" s="177"/>
+      <c r="F14" s="177"/>
+      <c r="G14" s="177"/>
+      <c r="H14" s="177"/>
+      <c r="I14" s="177"/>
+      <c r="J14" s="177"/>
+      <c r="K14" s="177"/>
+      <c r="L14" s="177"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="176"/>
-      <c r="B15" s="176"/>
-      <c r="C15" s="176"/>
-      <c r="D15" s="176"/>
-      <c r="E15" s="176"/>
-      <c r="F15" s="176"/>
-      <c r="G15" s="176"/>
-      <c r="H15" s="176"/>
-      <c r="I15" s="176"/>
-      <c r="J15" s="176"/>
-      <c r="K15" s="176"/>
-      <c r="L15" s="176"/>
+      <c r="A15" s="177"/>
+      <c r="B15" s="177"/>
+      <c r="C15" s="177"/>
+      <c r="D15" s="177"/>
+      <c r="E15" s="177"/>
+      <c r="F15" s="177"/>
+      <c r="G15" s="177"/>
+      <c r="H15" s="177"/>
+      <c r="I15" s="177"/>
+      <c r="J15" s="177"/>
+      <c r="K15" s="177"/>
+      <c r="L15" s="177"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="176"/>
-      <c r="B16" s="176"/>
-      <c r="C16" s="176"/>
-      <c r="D16" s="176"/>
-      <c r="E16" s="176"/>
-      <c r="F16" s="176"/>
-      <c r="G16" s="176"/>
-      <c r="H16" s="176"/>
-      <c r="I16" s="176"/>
-      <c r="J16" s="176"/>
-      <c r="K16" s="176"/>
-      <c r="L16" s="176"/>
+      <c r="A16" s="177"/>
+      <c r="B16" s="177"/>
+      <c r="C16" s="177"/>
+      <c r="D16" s="177"/>
+      <c r="E16" s="177"/>
+      <c r="F16" s="177"/>
+      <c r="G16" s="177"/>
+      <c r="H16" s="177"/>
+      <c r="I16" s="177"/>
+      <c r="J16" s="177"/>
+      <c r="K16" s="177"/>
+      <c r="L16" s="177"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="176"/>
-      <c r="B17" s="176"/>
-      <c r="C17" s="176"/>
-      <c r="D17" s="176"/>
-      <c r="E17" s="176"/>
-      <c r="F17" s="176"/>
-      <c r="G17" s="176"/>
-      <c r="H17" s="176"/>
-      <c r="I17" s="176"/>
-      <c r="J17" s="176"/>
-      <c r="K17" s="176"/>
-      <c r="L17" s="176"/>
+      <c r="A17" s="177"/>
+      <c r="B17" s="177"/>
+      <c r="C17" s="177"/>
+      <c r="D17" s="177"/>
+      <c r="E17" s="177"/>
+      <c r="F17" s="177"/>
+      <c r="G17" s="177"/>
+      <c r="H17" s="177"/>
+      <c r="I17" s="177"/>
+      <c r="J17" s="177"/>
+      <c r="K17" s="177"/>
+      <c r="L17" s="177"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="176"/>
-      <c r="B18" s="176"/>
-      <c r="C18" s="176"/>
-      <c r="D18" s="176"/>
-      <c r="E18" s="176"/>
-      <c r="F18" s="176"/>
-      <c r="G18" s="176"/>
-      <c r="H18" s="176"/>
-      <c r="I18" s="176"/>
-      <c r="J18" s="176"/>
-      <c r="K18" s="176"/>
-      <c r="L18" s="176"/>
+      <c r="A18" s="177"/>
+      <c r="B18" s="177"/>
+      <c r="C18" s="177"/>
+      <c r="D18" s="177"/>
+      <c r="E18" s="177"/>
+      <c r="F18" s="177"/>
+      <c r="G18" s="177"/>
+      <c r="H18" s="177"/>
+      <c r="I18" s="177"/>
+      <c r="J18" s="177"/>
+      <c r="K18" s="177"/>
+      <c r="L18" s="177"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="176"/>
-      <c r="B19" s="176"/>
-      <c r="C19" s="176"/>
-      <c r="D19" s="176"/>
-      <c r="E19" s="176"/>
-      <c r="F19" s="176"/>
-      <c r="G19" s="176"/>
-      <c r="H19" s="176"/>
-      <c r="I19" s="176"/>
-      <c r="J19" s="176"/>
-      <c r="K19" s="176"/>
-      <c r="L19" s="176"/>
+      <c r="A19" s="177"/>
+      <c r="B19" s="177"/>
+      <c r="C19" s="177"/>
+      <c r="D19" s="177"/>
+      <c r="E19" s="177"/>
+      <c r="F19" s="177"/>
+      <c r="G19" s="177"/>
+      <c r="H19" s="177"/>
+      <c r="I19" s="177"/>
+      <c r="J19" s="177"/>
+      <c r="K19" s="177"/>
+      <c r="L19" s="177"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="176"/>
-      <c r="B20" s="176"/>
-      <c r="C20" s="176"/>
-      <c r="D20" s="176"/>
-      <c r="E20" s="176"/>
-      <c r="F20" s="176"/>
-      <c r="G20" s="176"/>
-      <c r="H20" s="176"/>
-      <c r="I20" s="176"/>
-      <c r="J20" s="176"/>
-      <c r="K20" s="176"/>
-      <c r="L20" s="176"/>
+      <c r="A20" s="177"/>
+      <c r="B20" s="177"/>
+      <c r="C20" s="177"/>
+      <c r="D20" s="177"/>
+      <c r="E20" s="177"/>
+      <c r="F20" s="177"/>
+      <c r="G20" s="177"/>
+      <c r="H20" s="177"/>
+      <c r="I20" s="177"/>
+      <c r="J20" s="177"/>
+      <c r="K20" s="177"/>
+      <c r="L20" s="177"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="176"/>
-      <c r="B21" s="176"/>
-      <c r="C21" s="176"/>
-      <c r="D21" s="176"/>
-      <c r="E21" s="176"/>
-      <c r="F21" s="176"/>
-      <c r="G21" s="176"/>
-      <c r="H21" s="176"/>
-      <c r="I21" s="176"/>
-      <c r="J21" s="176"/>
-      <c r="K21" s="176"/>
-      <c r="L21" s="176"/>
+      <c r="A21" s="177"/>
+      <c r="B21" s="177"/>
+      <c r="C21" s="177"/>
+      <c r="D21" s="177"/>
+      <c r="E21" s="177"/>
+      <c r="F21" s="177"/>
+      <c r="G21" s="177"/>
+      <c r="H21" s="177"/>
+      <c r="I21" s="177"/>
+      <c r="J21" s="177"/>
+      <c r="K21" s="177"/>
+      <c r="L21" s="177"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="176"/>
-      <c r="B22" s="176"/>
-      <c r="C22" s="176"/>
-      <c r="D22" s="176"/>
-      <c r="E22" s="176"/>
-      <c r="F22" s="176"/>
-      <c r="G22" s="176"/>
-      <c r="H22" s="176"/>
-      <c r="I22" s="176"/>
-      <c r="J22" s="176"/>
-      <c r="K22" s="176"/>
-      <c r="L22" s="176"/>
+      <c r="A22" s="177"/>
+      <c r="B22" s="177"/>
+      <c r="C22" s="177"/>
+      <c r="D22" s="177"/>
+      <c r="E22" s="177"/>
+      <c r="F22" s="177"/>
+      <c r="G22" s="177"/>
+      <c r="H22" s="177"/>
+      <c r="I22" s="177"/>
+      <c r="J22" s="177"/>
+      <c r="K22" s="177"/>
+      <c r="L22" s="177"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="176"/>
-      <c r="B23" s="176"/>
-      <c r="C23" s="176"/>
-      <c r="D23" s="176"/>
-      <c r="E23" s="176"/>
-      <c r="F23" s="176"/>
-      <c r="G23" s="176"/>
-      <c r="H23" s="176"/>
-      <c r="I23" s="176"/>
-      <c r="J23" s="176"/>
-      <c r="K23" s="176"/>
-      <c r="L23" s="176"/>
+      <c r="A23" s="177"/>
+      <c r="B23" s="177"/>
+      <c r="C23" s="177"/>
+      <c r="D23" s="177"/>
+      <c r="E23" s="177"/>
+      <c r="F23" s="177"/>
+      <c r="G23" s="177"/>
+      <c r="H23" s="177"/>
+      <c r="I23" s="177"/>
+      <c r="J23" s="177"/>
+      <c r="K23" s="177"/>
+      <c r="L23" s="177"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="176"/>
-      <c r="B24" s="176"/>
-      <c r="C24" s="176"/>
-      <c r="D24" s="176"/>
-      <c r="E24" s="176"/>
-      <c r="F24" s="176"/>
-      <c r="G24" s="176"/>
-      <c r="H24" s="176"/>
-      <c r="I24" s="176"/>
-      <c r="J24" s="176"/>
-      <c r="K24" s="176"/>
-      <c r="L24" s="176"/>
+      <c r="A24" s="177"/>
+      <c r="B24" s="177"/>
+      <c r="C24" s="177"/>
+      <c r="D24" s="177"/>
+      <c r="E24" s="177"/>
+      <c r="F24" s="177"/>
+      <c r="G24" s="177"/>
+      <c r="H24" s="177"/>
+      <c r="I24" s="177"/>
+      <c r="J24" s="177"/>
+      <c r="K24" s="177"/>
+      <c r="L24" s="177"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="176"/>
-      <c r="B25" s="176"/>
-      <c r="C25" s="176"/>
-      <c r="D25" s="176"/>
-      <c r="E25" s="176"/>
-      <c r="F25" s="176"/>
-      <c r="G25" s="176"/>
-      <c r="H25" s="176"/>
-      <c r="I25" s="176"/>
-      <c r="J25" s="176"/>
-      <c r="K25" s="176"/>
-      <c r="L25" s="176"/>
+      <c r="A25" s="177"/>
+      <c r="B25" s="177"/>
+      <c r="C25" s="177"/>
+      <c r="D25" s="177"/>
+      <c r="E25" s="177"/>
+      <c r="F25" s="177"/>
+      <c r="G25" s="177"/>
+      <c r="H25" s="177"/>
+      <c r="I25" s="177"/>
+      <c r="J25" s="177"/>
+      <c r="K25" s="177"/>
+      <c r="L25" s="177"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="176"/>
-      <c r="B26" s="176"/>
-      <c r="C26" s="176"/>
-      <c r="D26" s="176"/>
-      <c r="E26" s="176"/>
-      <c r="F26" s="176"/>
-      <c r="G26" s="176"/>
-      <c r="H26" s="176"/>
-      <c r="I26" s="176"/>
-      <c r="J26" s="176"/>
-      <c r="K26" s="176"/>
-      <c r="L26" s="176"/>
+      <c r="A26" s="177"/>
+      <c r="B26" s="177"/>
+      <c r="C26" s="177"/>
+      <c r="D26" s="177"/>
+      <c r="E26" s="177"/>
+      <c r="F26" s="177"/>
+      <c r="G26" s="177"/>
+      <c r="H26" s="177"/>
+      <c r="I26" s="177"/>
+      <c r="J26" s="177"/>
+      <c r="K26" s="177"/>
+      <c r="L26" s="177"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" s="176"/>
-      <c r="B27" s="176"/>
-      <c r="C27" s="176"/>
-      <c r="D27" s="176"/>
-      <c r="E27" s="176"/>
-      <c r="F27" s="176"/>
-      <c r="G27" s="176"/>
-      <c r="H27" s="176"/>
-      <c r="I27" s="176"/>
-      <c r="J27" s="176"/>
-      <c r="K27" s="176"/>
-      <c r="L27" s="176"/>
+      <c r="A27" s="177"/>
+      <c r="B27" s="177"/>
+      <c r="C27" s="177"/>
+      <c r="D27" s="177"/>
+      <c r="E27" s="177"/>
+      <c r="F27" s="177"/>
+      <c r="G27" s="177"/>
+      <c r="H27" s="177"/>
+      <c r="I27" s="177"/>
+      <c r="J27" s="177"/>
+      <c r="K27" s="177"/>
+      <c r="L27" s="177"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" s="176"/>
-      <c r="B28" s="176"/>
-      <c r="C28" s="176"/>
-      <c r="D28" s="176"/>
-      <c r="E28" s="176"/>
-      <c r="F28" s="176"/>
-      <c r="G28" s="176"/>
-      <c r="H28" s="176"/>
-      <c r="I28" s="176"/>
-      <c r="J28" s="176"/>
-      <c r="K28" s="176"/>
-      <c r="L28" s="176"/>
+      <c r="A28" s="177"/>
+      <c r="B28" s="177"/>
+      <c r="C28" s="177"/>
+      <c r="D28" s="177"/>
+      <c r="E28" s="177"/>
+      <c r="F28" s="177"/>
+      <c r="G28" s="177"/>
+      <c r="H28" s="177"/>
+      <c r="I28" s="177"/>
+      <c r="J28" s="177"/>
+      <c r="K28" s="177"/>
+      <c r="L28" s="177"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" s="176"/>
-      <c r="B29" s="176"/>
-      <c r="C29" s="176"/>
-      <c r="D29" s="176"/>
-      <c r="E29" s="176"/>
-      <c r="F29" s="176"/>
-      <c r="G29" s="176"/>
-      <c r="H29" s="176"/>
-      <c r="I29" s="176"/>
-      <c r="J29" s="176"/>
-      <c r="K29" s="176"/>
-      <c r="L29" s="176"/>
+      <c r="A29" s="177"/>
+      <c r="B29" s="177"/>
+      <c r="C29" s="177"/>
+      <c r="D29" s="177"/>
+      <c r="E29" s="177"/>
+      <c r="F29" s="177"/>
+      <c r="G29" s="177"/>
+      <c r="H29" s="177"/>
+      <c r="I29" s="177"/>
+      <c r="J29" s="177"/>
+      <c r="K29" s="177"/>
+      <c r="L29" s="177"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="176"/>
-      <c r="B30" s="176"/>
-      <c r="C30" s="176"/>
-      <c r="D30" s="176"/>
-      <c r="E30" s="176"/>
-      <c r="F30" s="176"/>
-      <c r="G30" s="176"/>
-      <c r="H30" s="176"/>
-      <c r="I30" s="176"/>
-      <c r="J30" s="176"/>
-      <c r="K30" s="176"/>
-      <c r="L30" s="176"/>
+      <c r="A30" s="177"/>
+      <c r="B30" s="177"/>
+      <c r="C30" s="177"/>
+      <c r="D30" s="177"/>
+      <c r="E30" s="177"/>
+      <c r="F30" s="177"/>
+      <c r="G30" s="177"/>
+      <c r="H30" s="177"/>
+      <c r="I30" s="177"/>
+      <c r="J30" s="177"/>
+      <c r="K30" s="177"/>
+      <c r="L30" s="177"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="176"/>
-      <c r="B31" s="176"/>
-      <c r="C31" s="176"/>
-      <c r="D31" s="176"/>
-      <c r="E31" s="176"/>
-      <c r="F31" s="176"/>
-      <c r="G31" s="176"/>
-      <c r="H31" s="176"/>
-      <c r="I31" s="176"/>
-      <c r="J31" s="176"/>
-      <c r="K31" s="176"/>
-      <c r="L31" s="176"/>
+      <c r="A31" s="177"/>
+      <c r="B31" s="177"/>
+      <c r="C31" s="177"/>
+      <c r="D31" s="177"/>
+      <c r="E31" s="177"/>
+      <c r="F31" s="177"/>
+      <c r="G31" s="177"/>
+      <c r="H31" s="177"/>
+      <c r="I31" s="177"/>
+      <c r="J31" s="177"/>
+      <c r="K31" s="177"/>
+      <c r="L31" s="177"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32" s="176"/>
-      <c r="B32" s="176"/>
-      <c r="C32" s="176"/>
-      <c r="D32" s="176"/>
-      <c r="E32" s="176"/>
-      <c r="F32" s="176"/>
-      <c r="G32" s="176"/>
-      <c r="H32" s="176"/>
-      <c r="I32" s="176"/>
-      <c r="J32" s="176"/>
-      <c r="K32" s="176"/>
-      <c r="L32" s="176"/>
+      <c r="A32" s="177"/>
+      <c r="B32" s="177"/>
+      <c r="C32" s="177"/>
+      <c r="D32" s="177"/>
+      <c r="E32" s="177"/>
+      <c r="F32" s="177"/>
+      <c r="G32" s="177"/>
+      <c r="H32" s="177"/>
+      <c r="I32" s="177"/>
+      <c r="J32" s="177"/>
+      <c r="K32" s="177"/>
+      <c r="L32" s="177"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" s="176"/>
-      <c r="B33" s="176"/>
-      <c r="C33" s="176"/>
-      <c r="D33" s="176"/>
-      <c r="E33" s="176"/>
-      <c r="F33" s="176"/>
-      <c r="G33" s="176"/>
-      <c r="H33" s="176"/>
-      <c r="I33" s="176"/>
-      <c r="J33" s="176"/>
-      <c r="K33" s="176"/>
-      <c r="L33" s="176"/>
+      <c r="A33" s="177"/>
+      <c r="B33" s="177"/>
+      <c r="C33" s="177"/>
+      <c r="D33" s="177"/>
+      <c r="E33" s="177"/>
+      <c r="F33" s="177"/>
+      <c r="G33" s="177"/>
+      <c r="H33" s="177"/>
+      <c r="I33" s="177"/>
+      <c r="J33" s="177"/>
+      <c r="K33" s="177"/>
+      <c r="L33" s="177"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A34" s="176"/>
-      <c r="B34" s="176"/>
-      <c r="C34" s="176"/>
-      <c r="D34" s="176"/>
-      <c r="E34" s="176"/>
-      <c r="F34" s="176"/>
-      <c r="G34" s="176"/>
-      <c r="H34" s="176"/>
-      <c r="I34" s="176"/>
-      <c r="J34" s="176"/>
-      <c r="K34" s="176"/>
-      <c r="L34" s="176"/>
+      <c r="A34" s="177"/>
+      <c r="B34" s="177"/>
+      <c r="C34" s="177"/>
+      <c r="D34" s="177"/>
+      <c r="E34" s="177"/>
+      <c r="F34" s="177"/>
+      <c r="G34" s="177"/>
+      <c r="H34" s="177"/>
+      <c r="I34" s="177"/>
+      <c r="J34" s="177"/>
+      <c r="K34" s="177"/>
+      <c r="L34" s="177"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A35" s="176"/>
-      <c r="B35" s="176"/>
-      <c r="C35" s="176"/>
-      <c r="D35" s="176"/>
-      <c r="E35" s="176"/>
-      <c r="F35" s="176"/>
-      <c r="G35" s="176"/>
-      <c r="H35" s="176"/>
-      <c r="I35" s="176"/>
-      <c r="J35" s="176"/>
-      <c r="K35" s="176"/>
-      <c r="L35" s="176"/>
+      <c r="A35" s="177"/>
+      <c r="B35" s="177"/>
+      <c r="C35" s="177"/>
+      <c r="D35" s="177"/>
+      <c r="E35" s="177"/>
+      <c r="F35" s="177"/>
+      <c r="G35" s="177"/>
+      <c r="H35" s="177"/>
+      <c r="I35" s="177"/>
+      <c r="J35" s="177"/>
+      <c r="K35" s="177"/>
+      <c r="L35" s="177"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A36" s="176"/>
-      <c r="B36" s="176"/>
-      <c r="C36" s="176"/>
-      <c r="D36" s="176"/>
-      <c r="E36" s="176"/>
-      <c r="F36" s="176"/>
-      <c r="G36" s="176"/>
-      <c r="H36" s="176"/>
-      <c r="I36" s="176"/>
-      <c r="J36" s="176"/>
-      <c r="K36" s="176"/>
-      <c r="L36" s="176"/>
+      <c r="A36" s="177"/>
+      <c r="B36" s="177"/>
+      <c r="C36" s="177"/>
+      <c r="D36" s="177"/>
+      <c r="E36" s="177"/>
+      <c r="F36" s="177"/>
+      <c r="G36" s="177"/>
+      <c r="H36" s="177"/>
+      <c r="I36" s="177"/>
+      <c r="J36" s="177"/>
+      <c r="K36" s="177"/>
+      <c r="L36" s="177"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A37" s="176"/>
-      <c r="B37" s="176"/>
-      <c r="C37" s="176"/>
-      <c r="D37" s="176"/>
-      <c r="E37" s="176"/>
-      <c r="F37" s="176"/>
-      <c r="G37" s="176"/>
-      <c r="H37" s="176"/>
-      <c r="I37" s="176"/>
-      <c r="J37" s="176"/>
-      <c r="K37" s="176"/>
-      <c r="L37" s="176"/>
+      <c r="A37" s="177"/>
+      <c r="B37" s="177"/>
+      <c r="C37" s="177"/>
+      <c r="D37" s="177"/>
+      <c r="E37" s="177"/>
+      <c r="F37" s="177"/>
+      <c r="G37" s="177"/>
+      <c r="H37" s="177"/>
+      <c r="I37" s="177"/>
+      <c r="J37" s="177"/>
+      <c r="K37" s="177"/>
+      <c r="L37" s="177"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A38" s="176"/>
-      <c r="B38" s="176"/>
-      <c r="C38" s="176"/>
-      <c r="D38" s="176"/>
-      <c r="E38" s="176"/>
-      <c r="F38" s="176"/>
-      <c r="G38" s="176"/>
-      <c r="H38" s="176"/>
-      <c r="I38" s="176"/>
-      <c r="J38" s="176"/>
-      <c r="K38" s="176"/>
-      <c r="L38" s="176"/>
+      <c r="A38" s="177"/>
+      <c r="B38" s="177"/>
+      <c r="C38" s="177"/>
+      <c r="D38" s="177"/>
+      <c r="E38" s="177"/>
+      <c r="F38" s="177"/>
+      <c r="G38" s="177"/>
+      <c r="H38" s="177"/>
+      <c r="I38" s="177"/>
+      <c r="J38" s="177"/>
+      <c r="K38" s="177"/>
+      <c r="L38" s="177"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -6646,13 +6639,13 @@
     </row>
     <row r="10" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A10" s="115" t="s">
-        <v>922</v>
+        <v>919</v>
       </c>
       <c r="B10" s="115" t="s">
-        <v>923</v>
+        <v>920</v>
       </c>
       <c r="C10" s="116" t="s">
-        <v>924</v>
+        <v>921</v>
       </c>
       <c r="D10" s="115"/>
       <c r="E10" s="117"/>
@@ -6666,7 +6659,7 @@
         <v>703</v>
       </c>
       <c r="C11" s="116" t="s">
-        <v>960</v>
+        <v>957</v>
       </c>
       <c r="D11" s="115" t="s">
         <v>704</v>
@@ -6682,7 +6675,7 @@
         <v>705</v>
       </c>
       <c r="C12" s="116" t="s">
-        <v>918</v>
+        <v>915</v>
       </c>
       <c r="D12" s="115" t="s">
         <v>706</v>
@@ -6698,7 +6691,7 @@
         <v>707</v>
       </c>
       <c r="C13" s="116" t="s">
-        <v>919</v>
+        <v>916</v>
       </c>
       <c r="D13" s="115" t="s">
         <v>708</v>
@@ -6714,7 +6707,7 @@
         <v>709</v>
       </c>
       <c r="C14" s="116" t="s">
-        <v>920</v>
+        <v>917</v>
       </c>
       <c r="D14" s="115" t="s">
         <v>710</v>
@@ -6768,13 +6761,13 @@
     </row>
     <row r="18" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A18" s="115" t="s">
-        <v>922</v>
+        <v>919</v>
       </c>
       <c r="B18" s="115" t="s">
-        <v>921</v>
+        <v>918</v>
       </c>
       <c r="C18" s="116" t="s">
-        <v>935</v>
+        <v>932</v>
       </c>
       <c r="D18" s="115"/>
       <c r="E18" s="117"/>
@@ -6787,7 +6780,7 @@
         <v>720</v>
       </c>
       <c r="C19" s="116" t="s">
-        <v>936</v>
+        <v>933</v>
       </c>
       <c r="D19" s="115" t="s">
         <v>721</v>
@@ -6795,13 +6788,13 @@
       <c r="E19" s="117"/>
     </row>
     <row r="20" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="204" t="s">
+      <c r="A20" s="205" t="s">
         <v>722</v>
       </c>
-      <c r="B20" s="205"/>
-      <c r="C20" s="205"/>
-      <c r="D20" s="205"/>
-      <c r="E20" s="206"/>
+      <c r="B20" s="206"/>
+      <c r="C20" s="206"/>
+      <c r="D20" s="206"/>
+      <c r="E20" s="207"/>
     </row>
     <row r="21" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A21" s="118" t="s">
@@ -6834,13 +6827,13 @@
       <c r="E22" s="124"/>
     </row>
     <row r="23" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="207" t="s">
+      <c r="A23" s="208" t="s">
         <v>730</v>
       </c>
-      <c r="B23" s="208"/>
-      <c r="C23" s="209"/>
-      <c r="D23" s="208"/>
-      <c r="E23" s="210"/>
+      <c r="B23" s="209"/>
+      <c r="C23" s="210"/>
+      <c r="D23" s="209"/>
+      <c r="E23" s="211"/>
     </row>
     <row r="24" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="122" t="s">
@@ -6962,7 +6955,7 @@
         <v>746</v>
       </c>
       <c r="C31" s="47" t="s">
-        <v>904</v>
+        <v>901</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>747</v>
@@ -6971,13 +6964,13 @@
       <c r="F31" s="114"/>
     </row>
     <row r="32" spans="1:6" s="12" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="204" t="s">
+      <c r="A32" s="205" t="s">
         <v>748</v>
       </c>
-      <c r="B32" s="205"/>
-      <c r="C32" s="205"/>
-      <c r="D32" s="205"/>
-      <c r="E32" s="206"/>
+      <c r="B32" s="206"/>
+      <c r="C32" s="206"/>
+      <c r="D32" s="206"/>
+      <c r="E32" s="207"/>
     </row>
     <row r="33" spans="1:6" s="25" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A33" s="122" t="s">
@@ -7020,7 +7013,7 @@
         <v>755</v>
       </c>
       <c r="C35" s="47" t="s">
-        <v>910</v>
+        <v>907</v>
       </c>
       <c r="D35" s="96" t="s">
         <v>651</v>
@@ -7113,7 +7106,7 @@
         <v>772</v>
       </c>
       <c r="C41" s="123" t="s">
-        <v>1109</v>
+        <v>1106</v>
       </c>
       <c r="D41" s="101" t="s">
         <v>773</v>
@@ -7543,9 +7536,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E52C375-4A34-4943-A40B-CD02CAD0761B}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7587,7 +7580,7 @@
         <v>820</v>
       </c>
       <c r="C2" s="129" t="s">
-        <v>925</v>
+        <v>922</v>
       </c>
       <c r="D2" s="76" t="s">
         <v>821</v>
@@ -7613,11 +7606,11 @@
       <c r="A4" s="78" t="s">
         <v>485</v>
       </c>
-      <c r="B4" s="79" t="s">
-        <v>826</v>
+      <c r="B4" s="157" t="s">
+        <v>1171</v>
       </c>
       <c r="C4" s="136" t="s">
-        <v>926</v>
+        <v>923</v>
       </c>
       <c r="D4" s="79" t="s">
         <v>289</v>
@@ -7646,13 +7639,13 @@
         <v>168</v>
       </c>
       <c r="B6" s="79" t="s">
+        <v>826</v>
+      </c>
+      <c r="C6" s="136" t="s">
+        <v>922</v>
+      </c>
+      <c r="D6" s="79" t="s">
         <v>827</v>
-      </c>
-      <c r="C6" s="136" t="s">
-        <v>925</v>
-      </c>
-      <c r="D6" s="79" t="s">
-        <v>828</v>
       </c>
       <c r="E6" s="133"/>
     </row>
@@ -7661,10 +7654,10 @@
         <v>822</v>
       </c>
       <c r="B7" s="79" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="C7" s="136" t="s">
-        <v>982</v>
+        <v>979</v>
       </c>
       <c r="D7" s="157"/>
       <c r="E7" s="133"/>
@@ -7673,11 +7666,11 @@
       <c r="A8" s="78" t="s">
         <v>485</v>
       </c>
-      <c r="B8" s="79" t="s">
-        <v>830</v>
+      <c r="B8" s="157" t="s">
+        <v>1172</v>
       </c>
       <c r="C8" s="136" t="s">
-        <v>926</v>
+        <v>923</v>
       </c>
       <c r="D8" s="79" t="s">
         <v>289</v>
@@ -7706,13 +7699,13 @@
         <v>168</v>
       </c>
       <c r="B10" s="79" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="C10" s="136" t="s">
-        <v>925</v>
+        <v>922</v>
       </c>
       <c r="D10" s="79" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="E10" s="133"/>
     </row>
@@ -7721,23 +7714,23 @@
         <v>822</v>
       </c>
       <c r="B11" s="79" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="C11" s="136" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="D11" s="157"/>
       <c r="E11" s="133"/>
     </row>
     <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="78" t="s">
-        <v>14</v>
+      <c r="A12" s="158" t="s">
+        <v>485</v>
       </c>
       <c r="B12" s="79" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="C12" s="136" t="s">
-        <v>926</v>
+        <v>923</v>
       </c>
       <c r="D12" s="79" t="s">
         <v>289</v>
@@ -7766,10 +7759,10 @@
         <v>168</v>
       </c>
       <c r="B14" s="79" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="C14" s="136" t="s">
-        <v>947</v>
+        <v>944</v>
       </c>
       <c r="D14" s="79" t="s">
         <v>821</v>
@@ -7781,13 +7774,13 @@
         <v>822</v>
       </c>
       <c r="B15" s="79" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="C15" s="136" t="s">
-        <v>946</v>
+        <v>943</v>
       </c>
       <c r="D15" s="79" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="E15" s="133"/>
     </row>
@@ -7795,11 +7788,11 @@
       <c r="A16" s="78" t="s">
         <v>485</v>
       </c>
-      <c r="B16" s="79" t="s">
-        <v>838</v>
+      <c r="B16" s="157" t="s">
+        <v>1173</v>
       </c>
       <c r="C16" s="136" t="s">
-        <v>948</v>
+        <v>945</v>
       </c>
       <c r="D16" s="79" t="s">
         <v>289</v>
@@ -7852,24 +7845,24 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="211" t="s">
-        <v>1025</v>
-      </c>
-      <c r="B2" s="212"/>
-      <c r="C2" s="212"/>
-      <c r="D2" s="212"/>
-      <c r="E2" s="212"/>
-      <c r="F2" s="212"/>
+      <c r="A2" s="212" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B2" s="213"/>
+      <c r="C2" s="213"/>
+      <c r="D2" s="213"/>
+      <c r="E2" s="213"/>
+      <c r="F2" s="213"/>
     </row>
     <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>168</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>839</v>
+        <v>836</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -7877,10 +7870,10 @@
         <v>179</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="C4" s="44" t="s">
-        <v>939</v>
+        <v>936</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -7888,10 +7881,10 @@
         <v>174</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>842</v>
+        <v>839</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="80" x14ac:dyDescent="0.2">
@@ -7899,10 +7892,10 @@
         <v>179</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>938</v>
+        <v>935</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -7910,87 +7903,87 @@
         <v>174</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>847</v>
+        <v>844</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>929</v>
+        <v>926</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>850</v>
+        <v>847</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
+        <v>845</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>848</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>851</v>
-      </c>
       <c r="C10" s="5" t="s">
-        <v>852</v>
+        <v>849</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>853</v>
+        <v>850</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>854</v>
+        <v>851</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>855</v>
+        <v>852</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>856</v>
+        <v>853</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>857</v>
+        <v>854</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>858</v>
+        <v>855</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>859</v>
+        <v>856</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>928</v>
+        <v>925</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -7999,10 +7992,10 @@
         <v>614</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>860</v>
+        <v>857</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>861</v>
+        <v>858</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -8011,22 +8004,22 @@
         <v>14</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>862</v>
+        <v>859</v>
       </c>
       <c r="C16" s="59" t="s">
-        <v>863</v>
+        <v>860</v>
       </c>
       <c r="D16" s="15"/>
     </row>
     <row r="17" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>864</v>
+        <v>861</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>865</v>
+        <v>862</v>
       </c>
       <c r="C17" s="60" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="D17" s="15"/>
     </row>
@@ -8035,10 +8028,10 @@
         <v>325</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>1012</v>
+        <v>1009</v>
       </c>
       <c r="C18" s="161" t="s">
-        <v>1013</v>
+        <v>1010</v>
       </c>
       <c r="D18" s="162"/>
       <c r="E18" s="30"/>
@@ -8048,33 +8041,33 @@
         <v>325</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
       <c r="C19" s="161" t="s">
-        <v>1011</v>
+        <v>1008</v>
       </c>
       <c r="D19" s="162"/>
       <c r="E19" s="30"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="211" t="s">
-        <v>1014</v>
-      </c>
-      <c r="B20" s="212"/>
-      <c r="C20" s="212"/>
-      <c r="D20" s="212"/>
-      <c r="E20" s="212"/>
-      <c r="F20" s="212"/>
+      <c r="A20" s="212" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B20" s="213"/>
+      <c r="C20" s="213"/>
+      <c r="D20" s="213"/>
+      <c r="E20" s="213"/>
+      <c r="F20" s="213"/>
     </row>
     <row r="21" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>168</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>868</v>
+        <v>865</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="96" x14ac:dyDescent="0.2">
@@ -8082,13 +8075,13 @@
         <v>179</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>869</v>
+        <v>866</v>
       </c>
       <c r="C22" s="44" t="s">
-        <v>911</v>
+        <v>908</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>1146</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8096,10 +8089,10 @@
         <v>174</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>870</v>
+        <v>867</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -8107,206 +8100,206 @@
         <v>179</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>871</v>
+        <v>868</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>912</v>
+        <v>909</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="211" t="s">
-        <v>1015</v>
-      </c>
-      <c r="B25" s="212"/>
-      <c r="C25" s="212"/>
-      <c r="D25" s="212"/>
-      <c r="E25" s="212"/>
-      <c r="F25" s="212"/>
+      <c r="A25" s="212" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B25" s="213"/>
+      <c r="C25" s="213"/>
+      <c r="D25" s="213"/>
+      <c r="E25" s="213"/>
+      <c r="F25" s="213"/>
     </row>
     <row r="26" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>168</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>1017</v>
+        <v>1014</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="160" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>1029</v>
+        <v>1026</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>1018</v>
+        <v>1015</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>1145</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="211" t="s">
-        <v>1020</v>
-      </c>
-      <c r="B28" s="212"/>
-      <c r="C28" s="212"/>
-      <c r="D28" s="212"/>
-      <c r="E28" s="212"/>
-      <c r="F28" s="212"/>
+      <c r="A28" s="212" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B28" s="213"/>
+      <c r="C28" s="213"/>
+      <c r="D28" s="213"/>
+      <c r="E28" s="213"/>
+      <c r="F28" s="213"/>
     </row>
     <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>168</v>
       </c>
       <c r="B29" s="4" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>1021</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>1024</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="144" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>1029</v>
+        <v>1026</v>
       </c>
       <c r="B30" s="4" t="s">
+        <v>1020</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>1019</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>1141</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="212" t="s">
         <v>1023</v>
       </c>
-      <c r="C30" s="5" t="s">
-        <v>1022</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>1144</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="211" t="s">
-        <v>1026</v>
-      </c>
-      <c r="B31" s="212"/>
-      <c r="C31" s="212"/>
-      <c r="D31" s="212"/>
-      <c r="E31" s="212"/>
-      <c r="F31" s="212"/>
+      <c r="B31" s="213"/>
+      <c r="C31" s="213"/>
+      <c r="D31" s="213"/>
+      <c r="E31" s="213"/>
+      <c r="F31" s="213"/>
     </row>
     <row r="32" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>168</v>
       </c>
       <c r="B32" s="4" t="s">
+        <v>1024</v>
+      </c>
+      <c r="C32" s="5" t="s">
         <v>1027</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>1030</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="192" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
+        <v>1026</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>1025</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>1028</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="212" t="s">
         <v>1029</v>
       </c>
-      <c r="B33" s="4" t="s">
-        <v>1028</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>1031</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>1143</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="211" t="s">
-        <v>1032</v>
-      </c>
-      <c r="B34" s="212"/>
-      <c r="C34" s="212"/>
-      <c r="D34" s="212"/>
-      <c r="E34" s="212"/>
-      <c r="F34" s="212"/>
+      <c r="B34" s="213"/>
+      <c r="C34" s="213"/>
+      <c r="D34" s="213"/>
+      <c r="E34" s="213"/>
+      <c r="F34" s="213"/>
     </row>
     <row r="35" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>168</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>1035</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>1029</v>
+        <v>1026</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>1034</v>
+        <v>1031</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>1036</v>
+        <v>1033</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>1142</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="211" t="s">
-        <v>1042</v>
-      </c>
-      <c r="B37" s="212"/>
-      <c r="C37" s="212"/>
-      <c r="D37" s="212"/>
-      <c r="E37" s="212"/>
-      <c r="F37" s="212"/>
+      <c r="A37" s="212" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B37" s="213"/>
+      <c r="C37" s="213"/>
+      <c r="D37" s="213"/>
+      <c r="E37" s="213"/>
+      <c r="F37" s="213"/>
     </row>
     <row r="38" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>1029</v>
+        <v>1026</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>1039</v>
+        <v>1036</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>1045</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="211" t="s">
-        <v>1038</v>
-      </c>
-      <c r="B39" s="212"/>
-      <c r="C39" s="212"/>
-      <c r="D39" s="212"/>
-      <c r="E39" s="212"/>
-      <c r="F39" s="212"/>
+      <c r="A39" s="212" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B39" s="213"/>
+      <c r="C39" s="213"/>
+      <c r="D39" s="213"/>
+      <c r="E39" s="213"/>
+      <c r="F39" s="213"/>
     </row>
     <row r="40" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>168</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>1043</v>
+        <v>1040</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>1040</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="128" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>1029</v>
+        <v>1026</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>1044</v>
+        <v>1041</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>1041</v>
-      </c>
-      <c r="D41" s="213" t="s">
-        <v>1141</v>
+        <v>1038</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>1138</v>
       </c>
     </row>
   </sheetData>
@@ -8370,13 +8363,13 @@
         <v>7</v>
       </c>
       <c r="C2" s="84" t="s">
-        <v>1037</v>
+        <v>1034</v>
       </c>
       <c r="D2" s="82" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="83" t="s">
-        <v>1037</v>
+        <v>1034</v>
       </c>
       <c r="F2" s="82"/>
     </row>
@@ -8451,7 +8444,7 @@
     <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
-        <v>967</v>
+        <v>964</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>249</v>
@@ -9071,10 +9064,10 @@
     <row r="48" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="70"/>
       <c r="B48" s="141" t="s">
-        <v>940</v>
+        <v>937</v>
       </c>
       <c r="C48" s="142" t="s">
-        <v>941</v>
+        <v>938</v>
       </c>
       <c r="D48" s="70"/>
       <c r="E48" s="143"/>
@@ -9247,39 +9240,39 @@
     <row r="63" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A63" s="70"/>
       <c r="B63" s="141" t="s">
-        <v>943</v>
+        <v>940</v>
       </c>
       <c r="C63" s="142" t="s">
-        <v>944</v>
+        <v>941</v>
       </c>
       <c r="D63" s="70"/>
       <c r="E63" s="143"/>
       <c r="F63" s="144" t="s">
-        <v>945</v>
+        <v>942</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="70"/>
       <c r="B64" s="141" t="s">
-        <v>942</v>
+        <v>939</v>
       </c>
       <c r="C64" s="142" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="D64" s="70"/>
       <c r="E64" s="143"/>
     </row>
     <row r="65" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B65" s="1" t="s">
-        <v>879</v>
+        <v>876</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>880</v>
+        <v>877</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B66" s="1" t="s">
-        <v>881</v>
+        <v>878</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>62</v>
@@ -9287,32 +9280,32 @@
     </row>
     <row r="67" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B67" s="1" t="s">
-        <v>949</v>
+        <v>946</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>950</v>
+        <v>947</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B68" s="1" t="s">
-        <v>1046</v>
+        <v>1043</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>1047</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B69" s="1" t="s">
-        <v>1048</v>
+        <v>1045</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="70" spans="1:3" s="173" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="71" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>1112</v>
+        <v>1109</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>103</v>
@@ -9320,146 +9313,146 @@
     </row>
     <row r="72" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>1112</v>
+        <v>1109</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>1113</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>1112</v>
+        <v>1109</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>1114</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
+        <v>1109</v>
+      </c>
+      <c r="C74" s="2" t="s">
         <v>1112</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>1115</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>1112</v>
+        <v>1109</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>1116</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>1112</v>
+        <v>1109</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>1117</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>1112</v>
+        <v>1109</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>1130</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>1118</v>
+        <v>1115</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>1119</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>1118</v>
+        <v>1115</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>1120</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
+        <v>1115</v>
+      </c>
+      <c r="C80" s="2" t="s">
         <v>1118</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>1121</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>1118</v>
+        <v>1115</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>1122</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>1118</v>
+        <v>1115</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>1123</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>1118</v>
+        <v>1115</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>1124</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>1125</v>
+        <v>1122</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>1126</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>1125</v>
+        <v>1122</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>1127</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
+        <v>1122</v>
+      </c>
+      <c r="C86" s="2" t="s">
         <v>1125</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>1128</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>1125</v>
+        <v>1122</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>1129</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>1125</v>
+        <v>1122</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>1076</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>1125</v>
+        <v>1122</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>1086</v>
+        <v>1083</v>
       </c>
     </row>
   </sheetData>
@@ -9471,9 +9464,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9417505F-9ECE-441E-B1A9-0088F686151F}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:XFD6"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9525,45 +9518,45 @@
     </row>
     <row r="3" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>1161</v>
+        <v>1158</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>173</v>
       </c>
       <c r="C3" s="44" t="s">
-        <v>1168</v>
+        <v>1165</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>1169</v>
+        <v>1166</v>
       </c>
       <c r="E3" s="74"/>
       <c r="F3" s="61"/>
     </row>
     <row r="4" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>1161</v>
+        <v>1158</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>1162</v>
+        <v>1159</v>
       </c>
       <c r="C4" s="44" t="s">
-        <v>1172</v>
+        <v>1169</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>1173</v>
+        <v>1170</v>
       </c>
       <c r="E4" s="74"/>
       <c r="F4" s="61"/>
     </row>
     <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>1165</v>
+        <v>1162</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>1164</v>
+        <v>1161</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>1163</v>
+        <v>1160</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="74"/>
@@ -9571,16 +9564,16 @@
     </row>
     <row r="6" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
+        <v>1160</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>1164</v>
+      </c>
+      <c r="C6" s="44" t="s">
         <v>1163</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>1167</v>
-      </c>
-      <c r="C6" s="44" t="s">
-        <v>1166</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>1170</v>
       </c>
       <c r="E6" s="74"/>
       <c r="F6" s="61"/>
@@ -9615,7 +9608,7 @@
         <v>181</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>1171</v>
+        <v>1168</v>
       </c>
       <c r="E8" s="31"/>
       <c r="F8" s="4" t="s">
@@ -9779,10 +9772,10 @@
         <v>168</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>894</v>
+        <v>891</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>895</v>
+        <v>892</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="32"/>
@@ -9793,32 +9786,32 @@
         <v>320</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>896</v>
+        <v>893</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>897</v>
+        <v>894</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="32"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="177" t="s">
-        <v>898</v>
-      </c>
-      <c r="B4" s="178"/>
-      <c r="C4" s="178"/>
-      <c r="D4" s="178"/>
-      <c r="E4" s="179"/>
+      <c r="A4" s="178" t="s">
+        <v>895</v>
+      </c>
+      <c r="B4" s="179"/>
+      <c r="C4" s="179"/>
+      <c r="D4" s="179"/>
+      <c r="E4" s="180"/>
     </row>
     <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>168</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>899</v>
+        <v>896</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>901</v>
+        <v>898</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="32"/>
@@ -9828,58 +9821,58 @@
         <v>320</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>900</v>
+        <v>897</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>902</v>
+        <v>899</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="32"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="177" t="s">
-        <v>986</v>
-      </c>
-      <c r="B7" s="178"/>
-      <c r="C7" s="178"/>
-      <c r="D7" s="178"/>
-      <c r="E7" s="179"/>
+      <c r="A7" s="178" t="s">
+        <v>983</v>
+      </c>
+      <c r="B7" s="179"/>
+      <c r="C7" s="179"/>
+      <c r="D7" s="179"/>
+      <c r="E7" s="180"/>
     </row>
     <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>168</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>988</v>
+        <v>985</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>989</v>
+        <v>986</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="32"/>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>990</v>
+        <v>987</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>991</v>
+        <v>988</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>992</v>
+        <v>989</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="32"/>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>993</v>
+        <v>990</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>994</v>
+        <v>991</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>995</v>
+        <v>992</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="32"/>
@@ -9889,10 +9882,10 @@
         <v>168</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>987</v>
+        <v>984</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>996</v>
+        <v>993</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="32"/>
@@ -9902,10 +9895,10 @@
         <v>320</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>997</v>
+        <v>994</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>998</v>
+        <v>995</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="32"/>
@@ -10036,96 +10029,96 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="177" t="s">
-        <v>1050</v>
-      </c>
-      <c r="B2" s="178"/>
-      <c r="C2" s="178"/>
-      <c r="D2" s="178"/>
-      <c r="E2" s="179"/>
+      <c r="A2" s="178" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B2" s="179"/>
+      <c r="C2" s="179"/>
+      <c r="D2" s="179"/>
+      <c r="E2" s="180"/>
     </row>
     <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>1051</v>
+        <v>1048</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>1053</v>
+        <v>1050</v>
       </c>
       <c r="C3" s="163" t="s">
-        <v>1052</v>
+        <v>1049</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="32"/>
     </row>
-    <row r="4" spans="1:6" ht="160" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>1053</v>
+      </c>
+      <c r="C4" s="163" t="s">
         <v>1051</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>1056</v>
-      </c>
-      <c r="C4" s="163" t="s">
-        <v>1054</v>
-      </c>
       <c r="D4" s="4" t="s">
-        <v>1157</v>
+        <v>1154</v>
       </c>
       <c r="E4" s="32"/>
     </row>
     <row r="5" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>1051</v>
+        <v>1048</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>1057</v>
+        <v>1054</v>
       </c>
       <c r="C5" s="163" t="s">
-        <v>1055</v>
+        <v>1052</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>1158</v>
+        <v>1155</v>
       </c>
       <c r="E5" s="32"/>
     </row>
     <row r="6" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>1051</v>
+        <v>1048</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>1059</v>
+        <v>1056</v>
       </c>
       <c r="C6" s="163" t="s">
-        <v>1058</v>
+        <v>1055</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>1159</v>
+        <v>1156</v>
       </c>
       <c r="E6" s="32"/>
     </row>
     <row r="7" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>1051</v>
+        <v>1048</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>1060</v>
+        <v>1057</v>
       </c>
       <c r="C7" s="163" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>1160</v>
+        <v>1157</v>
       </c>
       <c r="E7" s="32"/>
     </row>
     <row r="8" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>1051</v>
+        <v>1048</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="C8" s="163" t="s">
-        <v>1063</v>
+        <v>1060</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="32"/>
@@ -10135,23 +10128,23 @@
         <v>168</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>1064</v>
+        <v>1061</v>
       </c>
       <c r="C9" s="163" t="s">
-        <v>1066</v>
+        <v>1063</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="32"/>
     </row>
     <row r="10" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>1051</v>
+        <v>1048</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>1065</v>
+        <v>1062</v>
       </c>
       <c r="C10" s="163" t="s">
-        <v>1067</v>
+        <v>1064</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="32"/>
@@ -10161,36 +10154,36 @@
         <v>174</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>1072</v>
+        <v>1069</v>
       </c>
       <c r="C11" s="163" t="s">
-        <v>1068</v>
+        <v>1065</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="32"/>
     </row>
     <row r="12" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>1071</v>
+        <v>1068</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>1073</v>
+        <v>1070</v>
       </c>
       <c r="C12" s="163" t="s">
-        <v>1069</v>
+        <v>1066</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="32"/>
     </row>
     <row r="13" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>1071</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>1074</v>
-      </c>
       <c r="C13" s="163" t="s">
-        <v>1070</v>
+        <v>1067</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="32"/>
@@ -10200,23 +10193,23 @@
         <v>174</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>1075</v>
+        <v>1072</v>
       </c>
       <c r="C14" s="163" t="s">
-        <v>1076</v>
+        <v>1073</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="32"/>
     </row>
     <row r="15" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>1077</v>
+        <v>1074</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>1078</v>
+        <v>1075</v>
       </c>
       <c r="C15" s="163" t="s">
-        <v>1079</v>
+        <v>1076</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="32"/>
@@ -10226,23 +10219,23 @@
         <v>14</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>1080</v>
+        <v>1077</v>
       </c>
       <c r="C16" s="163" t="s">
-        <v>1076</v>
+        <v>1073</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="32"/>
     </row>
     <row r="17" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>1071</v>
+        <v>1068</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>1084</v>
+        <v>1081</v>
       </c>
       <c r="C17" s="163" t="s">
-        <v>1081</v>
+        <v>1078</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="32"/>
@@ -10252,10 +10245,10 @@
         <v>14</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>1083</v>
+        <v>1080</v>
       </c>
       <c r="C18" s="163" t="s">
-        <v>1082</v>
+        <v>1079</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="32"/>
@@ -10265,10 +10258,10 @@
         <v>14</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>1085</v>
+        <v>1082</v>
       </c>
       <c r="C19" s="163" t="s">
-        <v>1086</v>
+        <v>1083</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="32"/>
@@ -10343,7 +10336,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>168</v>
       </c>
@@ -10363,7 +10356,7 @@
         <v>168</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>905</v>
+        <v>902</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>188</v>
@@ -10371,7 +10364,7 @@
       <c r="D3" s="4"/>
       <c r="E3" s="32"/>
     </row>
-    <row r="4" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>168</v>
       </c>
@@ -10397,10 +10390,10 @@
         <v>192</v>
       </c>
       <c r="C5" s="37" t="s">
-        <v>937</v>
+        <v>934</v>
       </c>
       <c r="D5" s="51" t="s">
-        <v>1154</v>
+        <v>1151</v>
       </c>
       <c r="E5" s="134"/>
       <c r="F5" s="1" t="s">
@@ -10418,10 +10411,10 @@
         <v>195</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>908</v>
+        <v>905</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
       <c r="E6" s="135"/>
       <c r="G6" s="52" t="s">
@@ -10436,10 +10429,10 @@
         <v>197</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>909</v>
+        <v>906</v>
       </c>
       <c r="D7" s="52" t="s">
-        <v>1156</v>
+        <v>1153</v>
       </c>
       <c r="E7" s="135"/>
       <c r="F7" s="53" t="s">
@@ -10479,7 +10472,7 @@
       </c>
       <c r="E9" s="41"/>
     </row>
-    <row r="10" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>206</v>
       </c>
@@ -10494,7 +10487,7 @@
       </c>
       <c r="E10" s="54"/>
     </row>
-    <row r="11" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>206</v>
       </c>
@@ -10509,7 +10502,7 @@
       </c>
       <c r="E11" s="40"/>
     </row>
-    <row r="12" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>206</v>
       </c>
@@ -10524,7 +10517,7 @@
       </c>
       <c r="E12" s="42"/>
     </row>
-    <row r="13" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>216</v>
       </c>
@@ -10542,7 +10535,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>216</v>
       </c>
@@ -10557,7 +10550,7 @@
       </c>
       <c r="E14" s="40"/>
     </row>
-    <row r="15" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>216</v>
       </c>
@@ -10572,7 +10565,7 @@
       </c>
       <c r="E15" s="38"/>
     </row>
-    <row r="16" spans="1:7" ht="64" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>216</v>
       </c>
@@ -10602,7 +10595,7 @@
       </c>
       <c r="E17" s="38"/>
     </row>
-    <row r="18" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>216</v>
       </c>
@@ -10617,13 +10610,13 @@
       </c>
       <c r="E18" s="38"/>
     </row>
-    <row r="19" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="6"/>
       <c r="B19" s="6" t="s">
         <v>236</v>
       </c>
       <c r="C19" s="49" t="s">
-        <v>903</v>
+        <v>900</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>237</v>
@@ -10633,10 +10626,10 @@
     <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="6"/>
       <c r="B20" s="6" t="s">
-        <v>1140</v>
+        <v>1137</v>
       </c>
       <c r="C20" s="174" t="s">
-        <v>1139</v>
+        <v>1136</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="175"/>
@@ -10657,7 +10650,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>28</v>
       </c>
@@ -10672,7 +10665,7 @@
       </c>
       <c r="E22" s="40"/>
     </row>
-    <row r="23" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>28</v>
       </c>
@@ -10752,35 +10745,35 @@
     </row>
     <row r="28" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>906</v>
+        <v>903</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>907</v>
+        <v>904</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>999</v>
+        <v>996</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="28"/>
     </row>
     <row r="29" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="177" t="s">
-        <v>1088</v>
-      </c>
-      <c r="B29" s="178"/>
-      <c r="C29" s="178"/>
-      <c r="D29" s="178"/>
-      <c r="E29" s="179"/>
+      <c r="A29" s="178" t="s">
+        <v>1085</v>
+      </c>
+      <c r="B29" s="179"/>
+      <c r="C29" s="179"/>
+      <c r="D29" s="179"/>
+      <c r="E29" s="180"/>
     </row>
     <row r="30" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>174</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>1087</v>
+        <v>1084</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>1089</v>
+        <v>1086</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="28"/>
@@ -10790,10 +10783,10 @@
         <v>174</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>1090</v>
+        <v>1087</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>1091</v>
+        <v>1088</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="28"/>
@@ -10803,10 +10796,10 @@
         <v>174</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>1092</v>
+        <v>1089</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>1093</v>
+        <v>1090</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="28"/>
@@ -10816,10 +10809,10 @@
         <v>614</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>1094</v>
+        <v>1091</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>1096</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -10827,21 +10820,21 @@
         <v>14</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>1095</v>
+        <v>1092</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>1097</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>1100</v>
+        <v>1097</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>1099</v>
+        <v>1096</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>1098</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -10849,10 +10842,10 @@
         <v>174</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>1102</v>
+        <v>1099</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>1101</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -10860,10 +10853,10 @@
         <v>614</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>1103</v>
+        <v>1100</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>1105</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -10871,26 +10864,26 @@
         <v>14</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>1104</v>
+        <v>1101</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>1106</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>1100</v>
+        <v>1097</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>1108</v>
+        <v>1105</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>1107</v>
+        <v>1104</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>1137</v>
+        <v>1134</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>208</v>
@@ -10898,56 +10891,56 @@
     </row>
     <row r="41" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>1137</v>
+        <v>1134</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>1131</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>1137</v>
+        <v>1134</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>1132</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>1137</v>
+        <v>1134</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>1133</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>1137</v>
+        <v>1134</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>1134</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>1137</v>
+        <v>1134</v>
       </c>
       <c r="C45" s="2" t="s">
+        <v>1132</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>1135</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>1138</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>1137</v>
+        <v>1134</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>1136</v>
+        <v>1133</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>1138</v>
+        <v>1135</v>
       </c>
     </row>
   </sheetData>
@@ -10999,13 +10992,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="183" t="s">
+      <c r="A2" s="181" t="s">
         <v>259</v>
       </c>
-      <c r="B2" s="184"/>
-      <c r="C2" s="184"/>
-      <c r="D2" s="184"/>
-      <c r="E2" s="185"/>
+      <c r="B2" s="182"/>
+      <c r="C2" s="182"/>
+      <c r="D2" s="182"/>
+      <c r="E2" s="183"/>
       <c r="F2" s="26"/>
     </row>
     <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -11093,10 +11086,10 @@
         <v>271</v>
       </c>
       <c r="B8" s="99" t="s">
-        <v>984</v>
+        <v>981</v>
       </c>
       <c r="C8" s="97" t="s">
-        <v>985</v>
+        <v>982</v>
       </c>
       <c r="D8" s="101"/>
       <c r="E8" s="100"/>
@@ -11133,13 +11126,13 @@
       <c r="F10" s="99"/>
     </row>
     <row r="11" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="186" t="s">
+      <c r="A11" s="184" t="s">
         <v>282</v>
       </c>
-      <c r="B11" s="187"/>
-      <c r="C11" s="187"/>
-      <c r="D11" s="187"/>
-      <c r="E11" s="188"/>
+      <c r="B11" s="185"/>
+      <c r="C11" s="185"/>
+      <c r="D11" s="185"/>
+      <c r="E11" s="186"/>
       <c r="F11" s="99"/>
     </row>
     <row r="12" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -11166,7 +11159,7 @@
         <v>286</v>
       </c>
       <c r="C13" s="131" t="s">
-        <v>882</v>
+        <v>879</v>
       </c>
       <c r="D13" s="68" t="s">
         <v>287</v>
@@ -11182,7 +11175,7 @@
         <v>288</v>
       </c>
       <c r="C14" s="132" t="s">
-        <v>883</v>
+        <v>880</v>
       </c>
       <c r="D14" s="72" t="s">
         <v>289</v>
@@ -11191,13 +11184,13 @@
       <c r="F14" s="70"/>
     </row>
     <row r="15" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="177" t="s">
+      <c r="A15" s="178" t="s">
         <v>290</v>
       </c>
-      <c r="B15" s="178"/>
-      <c r="C15" s="178"/>
-      <c r="D15" s="178"/>
-      <c r="E15" s="179"/>
+      <c r="B15" s="179"/>
+      <c r="C15" s="179"/>
+      <c r="D15" s="179"/>
+      <c r="E15" s="180"/>
       <c r="F15" s="99"/>
     </row>
     <row r="16" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -11249,13 +11242,13 @@
       <c r="F18" s="70"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="177" t="s">
-        <v>964</v>
-      </c>
-      <c r="B19" s="178"/>
-      <c r="C19" s="178"/>
-      <c r="D19" s="178"/>
-      <c r="E19" s="179"/>
+      <c r="A19" s="178" t="s">
+        <v>961</v>
+      </c>
+      <c r="B19" s="179"/>
+      <c r="C19" s="179"/>
+      <c r="D19" s="179"/>
+      <c r="E19" s="180"/>
       <c r="F19" s="99"/>
     </row>
     <row r="20" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -11263,10 +11256,10 @@
         <v>168</v>
       </c>
       <c r="B20" s="111" t="s">
-        <v>965</v>
+        <v>962</v>
       </c>
       <c r="C20" s="112" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
       <c r="D20" s="94"/>
       <c r="E20" s="110"/>
@@ -11277,13 +11270,13 @@
         <v>267</v>
       </c>
       <c r="B21" s="111" t="s">
-        <v>968</v>
+        <v>965</v>
       </c>
       <c r="C21" s="112" t="s">
-        <v>974</v>
-      </c>
-      <c r="D21" s="214" t="s">
-        <v>1150</v>
+        <v>971</v>
+      </c>
+      <c r="D21" s="176" t="s">
+        <v>1147</v>
       </c>
       <c r="E21" s="110"/>
       <c r="F21" s="99"/>
@@ -11293,41 +11286,41 @@
         <v>267</v>
       </c>
       <c r="B22" s="111" t="s">
-        <v>970</v>
+        <v>967</v>
       </c>
       <c r="C22" s="112" t="s">
-        <v>969</v>
+        <v>966</v>
       </c>
       <c r="D22" s="94" t="s">
-        <v>1149</v>
+        <v>1146</v>
       </c>
       <c r="E22" s="110"/>
       <c r="F22" s="99"/>
     </row>
     <row r="23" spans="1:6" s="156" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A23" s="150" t="s">
-        <v>973</v>
+        <v>970</v>
       </c>
       <c r="B23" s="151" t="s">
-        <v>971</v>
+        <v>968</v>
       </c>
       <c r="C23" s="152" t="s">
-        <v>972</v>
+        <v>969</v>
       </c>
       <c r="D23" s="153" t="s">
-        <v>1148</v>
+        <v>1145</v>
       </c>
       <c r="E23" s="154"/>
       <c r="F23" s="155"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="177" t="s">
+      <c r="A24" s="178" t="s">
         <v>304</v>
       </c>
-      <c r="B24" s="178"/>
-      <c r="C24" s="178"/>
-      <c r="D24" s="178"/>
-      <c r="E24" s="179"/>
+      <c r="B24" s="179"/>
+      <c r="C24" s="179"/>
+      <c r="D24" s="179"/>
+      <c r="E24" s="180"/>
       <c r="F24" s="99"/>
     </row>
     <row r="25" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -11395,13 +11388,13 @@
       <c r="F28" s="99"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="177" t="s">
+      <c r="A29" s="178" t="s">
         <v>316</v>
       </c>
-      <c r="B29" s="178"/>
-      <c r="C29" s="178"/>
-      <c r="D29" s="178"/>
-      <c r="E29" s="179"/>
+      <c r="B29" s="179"/>
+      <c r="C29" s="179"/>
+      <c r="D29" s="179"/>
+      <c r="E29" s="180"/>
       <c r="F29" s="99"/>
     </row>
     <row r="30" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -11425,10 +11418,10 @@
         <v>320</v>
       </c>
       <c r="B31" s="96" t="s">
-        <v>893</v>
+        <v>890</v>
       </c>
       <c r="C31" s="44" t="s">
-        <v>1110</v>
+        <v>1107</v>
       </c>
       <c r="D31" s="96"/>
       <c r="E31" s="100"/>
@@ -11442,10 +11435,10 @@
         <v>321</v>
       </c>
       <c r="C32" s="44" t="s">
-        <v>1111</v>
+        <v>1108</v>
       </c>
       <c r="D32" s="96" t="s">
-        <v>1151</v>
+        <v>1148</v>
       </c>
       <c r="E32" s="100"/>
       <c r="F32" s="99"/>
@@ -11521,13 +11514,13 @@
       <c r="F37" s="99"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="177" t="s">
+      <c r="A38" s="178" t="s">
         <v>330</v>
       </c>
-      <c r="B38" s="178"/>
-      <c r="C38" s="178"/>
-      <c r="D38" s="178"/>
-      <c r="E38" s="179"/>
+      <c r="B38" s="179"/>
+      <c r="C38" s="179"/>
+      <c r="D38" s="179"/>
+      <c r="E38" s="180"/>
       <c r="F38" s="99"/>
     </row>
     <row r="39" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -11554,7 +11547,7 @@
         <v>335</v>
       </c>
       <c r="C40" s="97" t="s">
-        <v>951</v>
+        <v>948</v>
       </c>
       <c r="D40" s="96" t="s">
         <v>336</v>
@@ -11583,23 +11576,23 @@
         <v>337</v>
       </c>
       <c r="B42" s="96" t="s">
-        <v>887</v>
+        <v>884</v>
       </c>
       <c r="C42" s="97" t="s">
-        <v>888</v>
+        <v>885</v>
       </c>
       <c r="D42" s="96"/>
       <c r="E42" s="100"/>
       <c r="F42" s="99"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="177" t="s">
+      <c r="A43" s="178" t="s">
         <v>341</v>
       </c>
-      <c r="B43" s="178"/>
-      <c r="C43" s="178"/>
-      <c r="D43" s="178"/>
-      <c r="E43" s="179"/>
+      <c r="B43" s="179"/>
+      <c r="C43" s="179"/>
+      <c r="D43" s="179"/>
+      <c r="E43" s="180"/>
       <c r="F43" s="99"/>
     </row>
     <row r="44" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -11619,13 +11612,13 @@
       <c r="F44" s="99"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="177" t="s">
+      <c r="A45" s="178" t="s">
         <v>345</v>
       </c>
-      <c r="B45" s="178"/>
-      <c r="C45" s="178"/>
-      <c r="D45" s="178"/>
-      <c r="E45" s="179"/>
+      <c r="B45" s="179"/>
+      <c r="C45" s="179"/>
+      <c r="D45" s="179"/>
+      <c r="E45" s="180"/>
       <c r="F45" s="99"/>
     </row>
     <row r="46" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -11649,10 +11642,10 @@
         <v>320</v>
       </c>
       <c r="B47" s="105" t="s">
-        <v>952</v>
+        <v>949</v>
       </c>
       <c r="C47" s="145" t="s">
-        <v>953</v>
+        <v>950</v>
       </c>
       <c r="D47" s="105"/>
       <c r="E47" s="110"/>
@@ -11762,7 +11755,7 @@
         <v>362</v>
       </c>
       <c r="C54" s="136" t="s">
-        <v>961</v>
+        <v>958</v>
       </c>
       <c r="D54" s="79" t="s">
         <v>289</v>
@@ -11771,13 +11764,13 @@
       <c r="F54" s="99"/>
     </row>
     <row r="55" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="177" t="s">
+      <c r="A55" s="178" t="s">
         <v>363</v>
       </c>
-      <c r="B55" s="178"/>
-      <c r="C55" s="178"/>
-      <c r="D55" s="178"/>
-      <c r="E55" s="179"/>
+      <c r="B55" s="179"/>
+      <c r="C55" s="179"/>
+      <c r="D55" s="179"/>
+      <c r="E55" s="180"/>
       <c r="F55" s="99"/>
     </row>
     <row r="56" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -11806,7 +11799,7 @@
         <v>367</v>
       </c>
       <c r="C57" s="97" t="s">
-        <v>917</v>
+        <v>914</v>
       </c>
       <c r="D57" s="96"/>
       <c r="E57" s="100"/>
@@ -11904,20 +11897,20 @@
         <v>380</v>
       </c>
       <c r="C64" s="97" t="s">
-        <v>916</v>
+        <v>913</v>
       </c>
       <c r="D64" s="96"/>
       <c r="E64" s="100"/>
       <c r="F64" s="99"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" s="177" t="s">
+      <c r="A65" s="178" t="s">
         <v>381</v>
       </c>
-      <c r="B65" s="178"/>
-      <c r="C65" s="178"/>
-      <c r="D65" s="178"/>
-      <c r="E65" s="179"/>
+      <c r="B65" s="179"/>
+      <c r="C65" s="179"/>
+      <c r="D65" s="179"/>
+      <c r="E65" s="180"/>
       <c r="F65" s="99"/>
     </row>
     <row r="66" spans="1:6" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -11946,7 +11939,7 @@
         <v>385</v>
       </c>
       <c r="C67" s="97" t="s">
-        <v>927</v>
+        <v>924</v>
       </c>
       <c r="D67" s="96"/>
       <c r="E67" s="100"/>
@@ -11975,7 +11968,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="137" t="s">
-        <v>930</v>
+        <v>927</v>
       </c>
       <c r="C69" s="77" t="s">
         <v>387</v>
@@ -11991,7 +11984,7 @@
         <v>68</v>
       </c>
       <c r="B70" s="137" t="s">
-        <v>931</v>
+        <v>928</v>
       </c>
       <c r="C70" s="77" t="s">
         <v>387</v>
@@ -12007,7 +12000,7 @@
         <v>68</v>
       </c>
       <c r="B71" s="138" t="s">
-        <v>932</v>
+        <v>929</v>
       </c>
       <c r="C71" s="139" t="s">
         <v>387</v>
@@ -12021,7 +12014,7 @@
         <v>68</v>
       </c>
       <c r="B72" s="138" t="s">
-        <v>933</v>
+        <v>930</v>
       </c>
       <c r="C72" s="139" t="s">
         <v>387</v>
@@ -12035,7 +12028,7 @@
         <v>68</v>
       </c>
       <c r="B73" s="138" t="s">
-        <v>934</v>
+        <v>931</v>
       </c>
       <c r="C73" s="139" t="s">
         <v>387</v>
@@ -12359,13 +12352,13 @@
       <c r="F95" s="99"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A96" s="177" t="s">
+      <c r="A96" s="178" t="s">
         <v>443</v>
       </c>
-      <c r="B96" s="178"/>
-      <c r="C96" s="178"/>
-      <c r="D96" s="178"/>
-      <c r="E96" s="179"/>
+      <c r="B96" s="179"/>
+      <c r="C96" s="179"/>
+      <c r="D96" s="179"/>
+      <c r="E96" s="180"/>
       <c r="F96" s="99"/>
     </row>
     <row r="97" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -12386,13 +12379,13 @@
     </row>
     <row r="98" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="96" t="s">
-        <v>954</v>
+        <v>951</v>
       </c>
       <c r="B98" s="96" t="s">
-        <v>956</v>
+        <v>953</v>
       </c>
       <c r="C98" s="97" t="s">
-        <v>955</v>
+        <v>952</v>
       </c>
       <c r="D98" s="96"/>
       <c r="E98" s="100"/>
@@ -12400,13 +12393,13 @@
     </row>
     <row r="99" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A99" s="96" t="s">
+        <v>951</v>
+      </c>
+      <c r="B99" s="96" t="s">
+        <v>955</v>
+      </c>
+      <c r="C99" s="97" t="s">
         <v>954</v>
-      </c>
-      <c r="B99" s="96" t="s">
-        <v>958</v>
-      </c>
-      <c r="C99" s="97" t="s">
-        <v>957</v>
       </c>
       <c r="D99" s="96"/>
       <c r="E99" s="100"/>
@@ -12487,13 +12480,13 @@
       <c r="F105" s="99"/>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A106" s="177" t="s">
+      <c r="A106" s="178" t="s">
         <v>453</v>
       </c>
-      <c r="B106" s="178"/>
-      <c r="C106" s="178"/>
-      <c r="D106" s="178"/>
-      <c r="E106" s="179"/>
+      <c r="B106" s="179"/>
+      <c r="C106" s="179"/>
+      <c r="D106" s="179"/>
+      <c r="E106" s="180"/>
       <c r="F106" s="99"/>
     </row>
     <row r="107" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -12520,7 +12513,7 @@
         <v>457</v>
       </c>
       <c r="C108" s="93" t="s">
-        <v>873</v>
+        <v>870</v>
       </c>
       <c r="D108" s="102" t="s">
         <v>458</v>
@@ -12561,13 +12554,13 @@
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A111" s="177" t="s">
+      <c r="A111" s="178" t="s">
         <v>465</v>
       </c>
-      <c r="B111" s="178"/>
-      <c r="C111" s="178"/>
-      <c r="D111" s="178"/>
-      <c r="E111" s="179"/>
+      <c r="B111" s="179"/>
+      <c r="C111" s="179"/>
+      <c r="D111" s="179"/>
+      <c r="E111" s="180"/>
       <c r="F111" s="99"/>
     </row>
     <row r="112" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -12578,7 +12571,7 @@
         <v>466</v>
       </c>
       <c r="C112" s="44" t="s">
-        <v>872</v>
+        <v>869</v>
       </c>
       <c r="D112" s="96" t="s">
         <v>467</v>
@@ -12605,10 +12598,10 @@
         <v>32</v>
       </c>
       <c r="B114" s="96" t="s">
-        <v>874</v>
+        <v>871</v>
       </c>
       <c r="C114" s="44" t="s">
-        <v>876</v>
+        <v>873</v>
       </c>
       <c r="D114" s="96"/>
       <c r="E114" s="100"/>
@@ -12619,10 +12612,10 @@
         <v>32</v>
       </c>
       <c r="B115" s="96" t="s">
-        <v>875</v>
+        <v>872</v>
       </c>
       <c r="C115" s="44" t="s">
-        <v>877</v>
+        <v>874</v>
       </c>
       <c r="D115" s="96"/>
       <c r="E115" s="100"/>
@@ -12657,13 +12650,13 @@
       <c r="F117" s="99"/>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A118" s="177" t="s">
+      <c r="A118" s="178" t="s">
         <v>475</v>
       </c>
-      <c r="B118" s="178"/>
-      <c r="C118" s="178"/>
-      <c r="D118" s="178"/>
-      <c r="E118" s="179"/>
+      <c r="B118" s="179"/>
+      <c r="C118" s="179"/>
+      <c r="D118" s="179"/>
+      <c r="E118" s="180"/>
       <c r="F118" s="99"/>
     </row>
     <row r="119" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -12743,13 +12736,13 @@
       <c r="F123" s="99"/>
     </row>
     <row r="124" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A124" s="180" t="s">
+      <c r="A124" s="187" t="s">
         <v>488</v>
       </c>
-      <c r="B124" s="181"/>
-      <c r="C124" s="181"/>
-      <c r="D124" s="181"/>
-      <c r="E124" s="182"/>
+      <c r="B124" s="188"/>
+      <c r="C124" s="188"/>
+      <c r="D124" s="188"/>
+      <c r="E124" s="189"/>
       <c r="F124" s="108" t="s">
         <v>491</v>
       </c>
@@ -12775,10 +12768,10 @@
         <v>168</v>
       </c>
       <c r="B126" s="96" t="s">
-        <v>1000</v>
+        <v>997</v>
       </c>
       <c r="C126" s="109" t="s">
-        <v>1001</v>
+        <v>998</v>
       </c>
       <c r="D126" s="94"/>
       <c r="E126" s="110"/>
@@ -12865,13 +12858,13 @@
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A132" s="177" t="s">
-        <v>975</v>
-      </c>
-      <c r="B132" s="178"/>
-      <c r="C132" s="178"/>
-      <c r="D132" s="178"/>
-      <c r="E132" s="179"/>
+      <c r="A132" s="178" t="s">
+        <v>972</v>
+      </c>
+      <c r="B132" s="179"/>
+      <c r="C132" s="179"/>
+      <c r="D132" s="179"/>
+      <c r="E132" s="180"/>
       <c r="F132" s="99"/>
     </row>
     <row r="133" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -12879,10 +12872,10 @@
         <v>168</v>
       </c>
       <c r="B133" s="111" t="s">
-        <v>976</v>
+        <v>973</v>
       </c>
       <c r="C133" s="112" t="s">
-        <v>975</v>
+        <v>972</v>
       </c>
       <c r="D133" s="94"/>
       <c r="E133" s="110"/>
@@ -12890,13 +12883,13 @@
     </row>
     <row r="134" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
-        <v>979</v>
+        <v>976</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>977</v>
+        <v>974</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>978</v>
+        <v>975</v>
       </c>
     </row>
     <row r="135" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -12904,23 +12897,23 @@
         <v>179</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>980</v>
+        <v>977</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>981</v>
+        <v>978</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>1152</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A136" s="177" t="s">
+      <c r="A136" s="178" t="s">
         <v>498</v>
       </c>
-      <c r="B136" s="178"/>
-      <c r="C136" s="178"/>
-      <c r="D136" s="178"/>
-      <c r="E136" s="179"/>
+      <c r="B136" s="179"/>
+      <c r="C136" s="179"/>
+      <c r="D136" s="179"/>
+      <c r="E136" s="180"/>
       <c r="F136" s="99"/>
     </row>
     <row r="137" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -12963,7 +12956,7 @@
         <v>503</v>
       </c>
       <c r="C139" s="136" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="D139" s="79" t="s">
         <v>289</v>
@@ -12979,7 +12972,7 @@
         <v>504</v>
       </c>
       <c r="C140" s="136" t="s">
-        <v>1003</v>
+        <v>1000</v>
       </c>
       <c r="D140" s="79" t="s">
         <v>289</v>
@@ -12995,7 +12988,7 @@
         <v>505</v>
       </c>
       <c r="C141" s="136" t="s">
-        <v>1004</v>
+        <v>1001</v>
       </c>
       <c r="D141" s="79" t="s">
         <v>289</v>
@@ -13037,28 +13030,28 @@
     </row>
     <row r="144" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A144" s="158" t="s">
-        <v>954</v>
+        <v>951</v>
       </c>
       <c r="B144" s="157" t="s">
-        <v>1005</v>
+        <v>1002</v>
       </c>
       <c r="C144" s="159" t="s">
-        <v>1006</v>
+        <v>1003</v>
       </c>
       <c r="D144" s="157" t="s">
-        <v>1153</v>
+        <v>1150</v>
       </c>
       <c r="E144" s="133"/>
       <c r="F144" s="99"/>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A145" s="177" t="s">
+      <c r="A145" s="178" t="s">
         <v>509</v>
       </c>
-      <c r="B145" s="178"/>
-      <c r="C145" s="178"/>
-      <c r="D145" s="178"/>
-      <c r="E145" s="179"/>
+      <c r="B145" s="179"/>
+      <c r="C145" s="179"/>
+      <c r="D145" s="179"/>
+      <c r="E145" s="180"/>
       <c r="F145" s="99"/>
     </row>
     <row r="146" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -13078,13 +13071,13 @@
       <c r="F146" s="99"/>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A147" s="177" t="s">
+      <c r="A147" s="178" t="s">
         <v>512</v>
       </c>
-      <c r="B147" s="178"/>
-      <c r="C147" s="178"/>
-      <c r="D147" s="178"/>
-      <c r="E147" s="179"/>
+      <c r="B147" s="179"/>
+      <c r="C147" s="179"/>
+      <c r="D147" s="179"/>
+      <c r="E147" s="180"/>
       <c r="F147" s="99"/>
     </row>
     <row r="148" spans="1:6" ht="64" x14ac:dyDescent="0.2">
@@ -13108,10 +13101,10 @@
         <v>320</v>
       </c>
       <c r="B149" s="96" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="C149" s="97" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
       <c r="D149" s="96"/>
       <c r="E149" s="100"/>
@@ -13141,7 +13134,7 @@
         <v>519</v>
       </c>
       <c r="C151" s="44" t="s">
-        <v>884</v>
+        <v>881</v>
       </c>
       <c r="D151" s="96" t="s">
         <v>520</v>
@@ -13154,23 +13147,23 @@
         <v>320</v>
       </c>
       <c r="B152" s="96" t="s">
-        <v>885</v>
+        <v>882</v>
       </c>
       <c r="C152" s="44" t="s">
-        <v>886</v>
+        <v>883</v>
       </c>
       <c r="D152" s="96"/>
       <c r="E152" s="100"/>
       <c r="F152" s="99"/>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A153" s="177" t="s">
+      <c r="A153" s="178" t="s">
         <v>521</v>
       </c>
-      <c r="B153" s="178"/>
-      <c r="C153" s="178"/>
-      <c r="D153" s="178"/>
-      <c r="E153" s="179"/>
+      <c r="B153" s="179"/>
+      <c r="C153" s="179"/>
+      <c r="D153" s="179"/>
+      <c r="E153" s="180"/>
       <c r="F153" s="99"/>
     </row>
     <row r="154" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -13225,7 +13218,7 @@
         <v>526</v>
       </c>
       <c r="C157" s="97" t="s">
-        <v>890</v>
+        <v>887</v>
       </c>
       <c r="D157" s="96"/>
       <c r="E157" s="100"/>
@@ -13236,7 +13229,7 @@
         <v>473</v>
       </c>
       <c r="B158" s="96" t="s">
-        <v>892</v>
+        <v>889</v>
       </c>
       <c r="C158" s="97" t="s">
         <v>37</v>
@@ -13250,23 +13243,23 @@
         <v>28</v>
       </c>
       <c r="B159" s="96" t="s">
-        <v>891</v>
+        <v>888</v>
       </c>
       <c r="C159" s="113" t="s">
-        <v>889</v>
+        <v>886</v>
       </c>
       <c r="D159" s="96"/>
       <c r="E159" s="100"/>
       <c r="F159" s="99"/>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A160" s="177" t="s">
+      <c r="A160" s="178" t="s">
         <v>527</v>
       </c>
-      <c r="B160" s="178"/>
-      <c r="C160" s="178"/>
-      <c r="D160" s="178"/>
-      <c r="E160" s="179"/>
+      <c r="B160" s="179"/>
+      <c r="C160" s="179"/>
+      <c r="D160" s="179"/>
+      <c r="E160" s="180"/>
       <c r="F160" s="99"/>
     </row>
     <row r="161" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -13318,13 +13311,13 @@
       <c r="F163" s="99"/>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A164" s="177" t="s">
+      <c r="A164" s="178" t="s">
         <v>535</v>
       </c>
-      <c r="B164" s="178"/>
-      <c r="C164" s="178"/>
-      <c r="D164" s="178"/>
-      <c r="E164" s="179"/>
+      <c r="B164" s="179"/>
+      <c r="C164" s="179"/>
+      <c r="D164" s="179"/>
+      <c r="E164" s="180"/>
       <c r="F164" s="99"/>
     </row>
     <row r="165" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -13365,7 +13358,7 @@
         <v>540</v>
       </c>
       <c r="C167" s="97" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="D167" s="96"/>
       <c r="E167" s="100"/>
@@ -13379,7 +13372,7 @@
         <v>541</v>
       </c>
       <c r="C168" s="97" t="s">
-        <v>1003</v>
+        <v>1000</v>
       </c>
       <c r="D168" s="96"/>
       <c r="E168" s="100"/>
@@ -13393,7 +13386,7 @@
         <v>542</v>
       </c>
       <c r="C169" s="97" t="s">
-        <v>1004</v>
+        <v>1001</v>
       </c>
       <c r="D169" s="96"/>
       <c r="E169" s="100"/>
@@ -13414,13 +13407,13 @@
       <c r="F170" s="99"/>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A171" s="177" t="s">
+      <c r="A171" s="178" t="s">
         <v>544</v>
       </c>
-      <c r="B171" s="178"/>
-      <c r="C171" s="178"/>
-      <c r="D171" s="178"/>
-      <c r="E171" s="179"/>
+      <c r="B171" s="179"/>
+      <c r="C171" s="179"/>
+      <c r="D171" s="179"/>
+      <c r="E171" s="180"/>
       <c r="F171" s="29"/>
     </row>
     <row r="172" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -13463,7 +13456,7 @@
         <v>551</v>
       </c>
       <c r="C174" s="44" t="s">
-        <v>910</v>
+        <v>907</v>
       </c>
       <c r="D174" s="96" t="s">
         <v>552</v>
@@ -14386,19 +14379,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A171:E171"/>
-    <mergeCell ref="A145:E145"/>
-    <mergeCell ref="A147:E147"/>
-    <mergeCell ref="A153:E153"/>
-    <mergeCell ref="A160:E160"/>
-    <mergeCell ref="A164:E164"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="A29:E29"/>
-    <mergeCell ref="A19:E19"/>
     <mergeCell ref="A136:E136"/>
     <mergeCell ref="A118:E118"/>
     <mergeCell ref="A43:E43"/>
@@ -14410,6 +14390,19 @@
     <mergeCell ref="A65:E65"/>
     <mergeCell ref="A124:E124"/>
     <mergeCell ref="A132:E132"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A29:E29"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A171:E171"/>
+    <mergeCell ref="A145:E145"/>
+    <mergeCell ref="A147:E147"/>
+    <mergeCell ref="A153:E153"/>
+    <mergeCell ref="A160:E160"/>
+    <mergeCell ref="A164:E164"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14456,13 +14449,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="192" t="s">
+      <c r="A2" s="193" t="s">
         <v>582</v>
       </c>
-      <c r="B2" s="193"/>
-      <c r="C2" s="193"/>
-      <c r="D2" s="193"/>
-      <c r="E2" s="194"/>
+      <c r="B2" s="194"/>
+      <c r="C2" s="194"/>
+      <c r="D2" s="194"/>
+      <c r="E2" s="195"/>
     </row>
     <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
@@ -14522,10 +14515,10 @@
     </row>
     <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B8" s="146" t="s">
-        <v>962</v>
+        <v>959</v>
       </c>
       <c r="C8" s="147" t="s">
-        <v>963</v>
+        <v>960</v>
       </c>
       <c r="D8" s="146"/>
       <c r="E8" s="148"/>
@@ -14580,15 +14573,15 @@
       </c>
     </row>
     <row r="13" spans="1:6" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="192" t="s">
+      <c r="A13" s="193" t="s">
         <v>598</v>
       </c>
-      <c r="B13" s="193"/>
-      <c r="C13" s="193"/>
-      <c r="D13" s="193"/>
-      <c r="E13" s="194"/>
-    </row>
-    <row r="14" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="B13" s="194"/>
+      <c r="C13" s="194"/>
+      <c r="D13" s="194"/>
+      <c r="E13" s="195"/>
+    </row>
+    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>168</v>
       </c>
@@ -14652,7 +14645,7 @@
         <v>609</v>
       </c>
       <c r="C18" s="129" t="s">
-        <v>878</v>
+        <v>875</v>
       </c>
       <c r="D18" s="76" t="s">
         <v>604</v>
@@ -14660,13 +14653,13 @@
       <c r="E18" s="130"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="201" t="s">
+      <c r="A19" s="202" t="s">
         <v>610</v>
       </c>
-      <c r="B19" s="202"/>
-      <c r="C19" s="202"/>
-      <c r="D19" s="202"/>
-      <c r="E19" s="203"/>
+      <c r="B19" s="203"/>
+      <c r="C19" s="203"/>
+      <c r="D19" s="203"/>
+      <c r="E19" s="204"/>
     </row>
     <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
@@ -14702,19 +14695,19 @@
         <v>618</v>
       </c>
       <c r="C22" s="66" t="s">
-        <v>959</v>
+        <v>956</v>
       </c>
       <c r="D22" s="64"/>
       <c r="E22" s="65"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="198" t="s">
+      <c r="A23" s="199" t="s">
         <v>619</v>
       </c>
-      <c r="B23" s="199"/>
-      <c r="C23" s="199"/>
-      <c r="D23" s="199"/>
-      <c r="E23" s="200"/>
+      <c r="B23" s="200"/>
+      <c r="C23" s="200"/>
+      <c r="D23" s="200"/>
+      <c r="E23" s="201"/>
     </row>
     <row r="24" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
@@ -14729,13 +14722,13 @@
       <c r="D24" s="15"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="189" t="s">
+      <c r="A25" s="190" t="s">
         <v>622</v>
       </c>
-      <c r="B25" s="190"/>
-      <c r="C25" s="190"/>
-      <c r="D25" s="190"/>
-      <c r="E25" s="191"/>
+      <c r="B25" s="191"/>
+      <c r="C25" s="191"/>
+      <c r="D25" s="191"/>
+      <c r="E25" s="192"/>
     </row>
     <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
@@ -14750,13 +14743,13 @@
       <c r="D26" s="15"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="189" t="s">
+      <c r="A27" s="190" t="s">
         <v>625</v>
       </c>
-      <c r="B27" s="190"/>
-      <c r="C27" s="190"/>
-      <c r="D27" s="190"/>
-      <c r="E27" s="191"/>
+      <c r="B27" s="191"/>
+      <c r="C27" s="191"/>
+      <c r="D27" s="191"/>
+      <c r="E27" s="192"/>
     </row>
     <row r="28" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A28" s="75" t="s">
@@ -14776,7 +14769,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" s="78" t="s">
         <v>614</v>
       </c>
@@ -14802,7 +14795,7 @@
         <v>635</v>
       </c>
       <c r="D30" s="157" t="s">
-        <v>1147</v>
+        <v>1144</v>
       </c>
       <c r="E30" s="73"/>
     </row>
@@ -14814,7 +14807,7 @@
         <v>636</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>913</v>
+        <v>910</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -14822,13 +14815,13 @@
         <v>179</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>914</v>
+        <v>911</v>
       </c>
       <c r="C32" s="18" t="s">
-        <v>915</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="16" t="s">
         <v>32</v>
       </c>
@@ -14843,15 +14836,15 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34" s="189" t="s">
+      <c r="A34" s="190" t="s">
         <v>640</v>
       </c>
-      <c r="B34" s="190"/>
-      <c r="C34" s="190"/>
-      <c r="D34" s="190"/>
-      <c r="E34" s="191"/>
-    </row>
-    <row r="35" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="B34" s="191"/>
+      <c r="C34" s="191"/>
+      <c r="D34" s="191"/>
+      <c r="E34" s="192"/>
+    </row>
+    <row r="35" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A35" s="16" t="s">
         <v>168</v>
       </c>
@@ -14866,13 +14859,13 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="195" t="s">
+      <c r="A36" s="196" t="s">
         <v>644</v>
       </c>
-      <c r="B36" s="196"/>
-      <c r="C36" s="196"/>
-      <c r="D36" s="196"/>
-      <c r="E36" s="197"/>
+      <c r="B36" s="197"/>
+      <c r="C36" s="197"/>
+      <c r="D36" s="197"/>
+      <c r="E36" s="198"/>
     </row>
     <row r="37" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A37" s="96" t="s">
@@ -14891,7 +14884,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A38" s="96" t="s">
         <v>260</v>
       </c>
@@ -14905,7 +14898,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="96" t="s">
         <v>179</v>
       </c>
@@ -14913,13 +14906,13 @@
         <v>650</v>
       </c>
       <c r="C39" s="47" t="s">
-        <v>910</v>
+        <v>907</v>
       </c>
       <c r="D39" s="96" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A40" s="96" t="s">
         <v>271</v>
       </c>
@@ -14933,7 +14926,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="96" t="s">
         <v>271</v>
       </c>
@@ -14947,7 +14940,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="96" t="s">
         <v>271</v>
       </c>
@@ -14961,7 +14954,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="96" t="s">
         <v>271</v>
       </c>
@@ -15001,7 +14994,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="16" t="s">
         <v>667</v>
       </c>
@@ -15018,7 +15011,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A47" s="16" t="s">
         <v>667</v>
       </c>
@@ -15035,7 +15028,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="96" t="s">
         <v>271</v>
       </c>
@@ -15052,7 +15045,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="96" t="s">
         <v>271</v>
       </c>
@@ -15085,47 +15078,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <SharedWithUsers xmlns="bf601f31-63a1-4825-9216-91d773c5ef9c">
-      <UserInfo>
-        <DisplayName>Erika Osti</DisplayName>
-        <AccountId>534</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Penny Johnson</DisplayName>
-        <AccountId>489</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Ben Childs</DisplayName>
-        <AccountId>643</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Thomas Leeds</DisplayName>
-        <AccountId>459</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Kasmyn Chen</DisplayName>
-        <AccountId>532</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="2799d30d-6731-4efe-ac9b-c4895a8828d9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010096D84A54A9CD274097F17166F184737D" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2fd95a4cfdf4f2f51219070f5dff16a8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="565e1b1d-057e-4d85-b896-01a5881d8a45" xmlns:ns3="bf601f31-63a1-4825-9216-91d773c5ef9c" xmlns:ns4="2799d30d-6731-4efe-ac9b-c4895a8828d9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f7499f6f4dc8ad2a533df04863f63fa7" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -15402,6 +15354,47 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <SharedWithUsers xmlns="bf601f31-63a1-4825-9216-91d773c5ef9c">
+      <UserInfo>
+        <DisplayName>Erika Osti</DisplayName>
+        <AccountId>534</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Penny Johnson</DisplayName>
+        <AccountId>489</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Ben Childs</DisplayName>
+        <AccountId>643</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Thomas Leeds</DisplayName>
+        <AccountId>459</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Kasmyn Chen</DisplayName>
+        <AccountId>532</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="2799d30d-6731-4efe-ac9b-c4895a8828d9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -15412,19 +15405,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="565e1b1d-057e-4d85-b896-01a5881d8a45"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="bf601f31-63a1-4825-9216-91d773c5ef9c"/>
-    <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAFDB110-4046-4E72-A1EF-1908ABEC3151}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15445,6 +15425,19 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="565e1b1d-057e-4d85-b896-01a5881d8a45"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="bf601f31-63a1-4825-9216-91d773c5ef9c"/>
+    <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Adding in the bilingual logic for toggles at the top of the dashboard etc.
</commit_message>
<xml_diff>
--- a/app/data/MCCD-localisation-V01.xlsx
+++ b/app/data/MCCD-localisation-V01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JALAT/GIT/medical-certificate-of-cause-of-death/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC288FEB-3F7A-1A4F-8D3B-7D120D1DDD8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD4268A3-2413-E047-9BAE-BBFA20734ABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13940" firstSheet="3" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13940" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Using this document" sheetId="8" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1747" uniqueCount="1174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1755" uniqueCount="1182">
   <si>
     <r>
       <rPr>
@@ -4469,6 +4469,30 @@
   </si>
   <si>
     <t>meoDeclarationSubmitForScrutinyCTA</t>
+  </si>
+  <si>
+    <t>dashboardToggleBilingual</t>
+  </si>
+  <si>
+    <t>You are currently using the bilingual service. New MCCDs will have the ability to be completed in both English and Welsh.</t>
+  </si>
+  <si>
+    <t>dashboardToggleBilingualLink</t>
+  </si>
+  <si>
+    <t>Switch to English only service</t>
+  </si>
+  <si>
+    <t>dashboardToggleMonolingual</t>
+  </si>
+  <si>
+    <t>You are currently using the English only service, but have previously used the bilingual service. New MCCDs will be completed in English only.</t>
+  </si>
+  <si>
+    <t>dashboardToggleMonolingualLink</t>
+  </si>
+  <si>
+    <t>Switch to bilingual service</t>
   </si>
 </sst>
 </file>
@@ -5499,6 +5523,15 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -5515,15 +5548,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -7536,7 +7560,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E52C375-4A34-4943-A40B-CD02CAD0761B}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
@@ -10297,11 +10321,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{344327F7-D7B0-4B8B-A26A-307F32EA23BD}">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10941,6 +10965,38 @@
       </c>
       <c r="D46" s="1" t="s">
         <v>1135</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+      <c r="B47" s="1" t="s">
+        <v>1174</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>1175</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="B48" s="1" t="s">
+        <v>1176</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" ht="64" x14ac:dyDescent="0.2">
+      <c r="B49" s="1" t="s">
+        <v>1178</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="B50" s="1" t="s">
+        <v>1180</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>1181</v>
       </c>
     </row>
   </sheetData>
@@ -10992,13 +11048,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="181" t="s">
+      <c r="A2" s="184" t="s">
         <v>259</v>
       </c>
-      <c r="B2" s="182"/>
-      <c r="C2" s="182"/>
-      <c r="D2" s="182"/>
-      <c r="E2" s="183"/>
+      <c r="B2" s="185"/>
+      <c r="C2" s="185"/>
+      <c r="D2" s="185"/>
+      <c r="E2" s="186"/>
       <c r="F2" s="26"/>
     </row>
     <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -11126,13 +11182,13 @@
       <c r="F10" s="99"/>
     </row>
     <row r="11" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="184" t="s">
+      <c r="A11" s="187" t="s">
         <v>282</v>
       </c>
-      <c r="B11" s="185"/>
-      <c r="C11" s="185"/>
-      <c r="D11" s="185"/>
-      <c r="E11" s="186"/>
+      <c r="B11" s="188"/>
+      <c r="C11" s="188"/>
+      <c r="D11" s="188"/>
+      <c r="E11" s="189"/>
       <c r="F11" s="99"/>
     </row>
     <row r="12" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -12736,13 +12792,13 @@
       <c r="F123" s="99"/>
     </row>
     <row r="124" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A124" s="187" t="s">
+      <c r="A124" s="181" t="s">
         <v>488</v>
       </c>
-      <c r="B124" s="188"/>
-      <c r="C124" s="188"/>
-      <c r="D124" s="188"/>
-      <c r="E124" s="189"/>
+      <c r="B124" s="182"/>
+      <c r="C124" s="182"/>
+      <c r="D124" s="182"/>
+      <c r="E124" s="183"/>
       <c r="F124" s="108" t="s">
         <v>491</v>
       </c>
@@ -14379,6 +14435,19 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A171:E171"/>
+    <mergeCell ref="A145:E145"/>
+    <mergeCell ref="A147:E147"/>
+    <mergeCell ref="A153:E153"/>
+    <mergeCell ref="A160:E160"/>
+    <mergeCell ref="A164:E164"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A29:E29"/>
+    <mergeCell ref="A19:E19"/>
     <mergeCell ref="A136:E136"/>
     <mergeCell ref="A118:E118"/>
     <mergeCell ref="A43:E43"/>
@@ -14390,19 +14459,6 @@
     <mergeCell ref="A65:E65"/>
     <mergeCell ref="A124:E124"/>
     <mergeCell ref="A132:E132"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="A29:E29"/>
-    <mergeCell ref="A19:E19"/>
-    <mergeCell ref="A171:E171"/>
-    <mergeCell ref="A145:E145"/>
-    <mergeCell ref="A147:E147"/>
-    <mergeCell ref="A153:E153"/>
-    <mergeCell ref="A160:E160"/>
-    <mergeCell ref="A164:E164"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15078,6 +15134,47 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <SharedWithUsers xmlns="bf601f31-63a1-4825-9216-91d773c5ef9c">
+      <UserInfo>
+        <DisplayName>Erika Osti</DisplayName>
+        <AccountId>534</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Penny Johnson</DisplayName>
+        <AccountId>489</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Ben Childs</DisplayName>
+        <AccountId>643</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Thomas Leeds</DisplayName>
+        <AccountId>459</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Kasmyn Chen</DisplayName>
+        <AccountId>532</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="2799d30d-6731-4efe-ac9b-c4895a8828d9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010096D84A54A9CD274097F17166F184737D" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2fd95a4cfdf4f2f51219070f5dff16a8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="565e1b1d-057e-4d85-b896-01a5881d8a45" xmlns:ns3="bf601f31-63a1-4825-9216-91d773c5ef9c" xmlns:ns4="2799d30d-6731-4efe-ac9b-c4895a8828d9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f7499f6f4dc8ad2a533df04863f63fa7" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -15354,47 +15451,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <SharedWithUsers xmlns="bf601f31-63a1-4825-9216-91d773c5ef9c">
-      <UserInfo>
-        <DisplayName>Erika Osti</DisplayName>
-        <AccountId>534</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Penny Johnson</DisplayName>
-        <AccountId>489</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Ben Childs</DisplayName>
-        <AccountId>643</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Thomas Leeds</DisplayName>
-        <AccountId>459</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Kasmyn Chen</DisplayName>
-        <AccountId>532</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="2799d30d-6731-4efe-ac9b-c4895a8828d9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -15405,6 +15461,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="565e1b1d-057e-4d85-b896-01a5881d8a45"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="bf601f31-63a1-4825-9216-91d773c5ef9c"/>
+    <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAFDB110-4046-4E72-A1EF-1908ABEC3151}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15425,19 +15494,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="565e1b1d-057e-4d85-b896-01a5881d8a45"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="bf601f31-63a1-4825-9216-91d773c5ef9c"/>
-    <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Updating the text on the bilingual toggle.
</commit_message>
<xml_diff>
--- a/app/data/MCCD-localisation-V01.xlsx
+++ b/app/data/MCCD-localisation-V01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JALAT/GIT/medical-certificate-of-cause-of-death/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD4268A3-2413-E047-9BAE-BBFA20734ABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3BDC830-AD1D-FC4E-A624-B949FDC350FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13940" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4474,25 +4474,25 @@
     <t>dashboardToggleBilingual</t>
   </si>
   <si>
-    <t>You are currently using the bilingual service. New MCCDs will have the ability to be completed in both English and Welsh.</t>
-  </si>
-  <si>
     <t>dashboardToggleBilingualLink</t>
   </si>
   <si>
-    <t>Switch to English only service</t>
-  </si>
-  <si>
     <t>dashboardToggleMonolingual</t>
   </si>
   <si>
-    <t>You are currently using the English only service, but have previously used the bilingual service. New MCCDs will be completed in English only.</t>
-  </si>
-  <si>
     <t>dashboardToggleMonolingualLink</t>
   </si>
   <si>
     <t>Switch to bilingual service</t>
+  </si>
+  <si>
+    <t>This is the bilingual MCCD service. New MCCDs can be completed in Welsh and English, or in English only.</t>
+  </si>
+  <si>
+    <t>Switch to English language service</t>
+  </si>
+  <si>
+    <t>This is the English language MCCD service, all fields must be completed in English. You previously created an MCCD using the bilingual Welsh and English MCCD service.</t>
   </si>
 </sst>
 </file>
@@ -5523,6 +5523,24 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -5530,24 +5548,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -10325,7 +10325,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D49" sqref="D49"/>
+      <selection pane="bottomLeft" activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10967,36 +10967,36 @@
         <v>1135</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
         <v>1174</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>1175</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B48" s="1" t="s">
+        <v>1175</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>1180</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" ht="80" x14ac:dyDescent="0.2">
+      <c r="B49" s="1" t="s">
         <v>1176</v>
       </c>
-      <c r="C48" s="2" t="s">
-        <v>1177</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3" ht="64" x14ac:dyDescent="0.2">
-      <c r="B49" s="1" t="s">
-        <v>1178</v>
-      </c>
       <c r="C49" s="2" t="s">
-        <v>1179</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="50" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B50" s="1" t="s">
-        <v>1180</v>
+        <v>1177</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>1181</v>
+        <v>1178</v>
       </c>
     </row>
   </sheetData>
@@ -11048,13 +11048,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="184" t="s">
+      <c r="A2" s="181" t="s">
         <v>259</v>
       </c>
-      <c r="B2" s="185"/>
-      <c r="C2" s="185"/>
-      <c r="D2" s="185"/>
-      <c r="E2" s="186"/>
+      <c r="B2" s="182"/>
+      <c r="C2" s="182"/>
+      <c r="D2" s="182"/>
+      <c r="E2" s="183"/>
       <c r="F2" s="26"/>
     </row>
     <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -11182,13 +11182,13 @@
       <c r="F10" s="99"/>
     </row>
     <row r="11" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="187" t="s">
+      <c r="A11" s="184" t="s">
         <v>282</v>
       </c>
-      <c r="B11" s="188"/>
-      <c r="C11" s="188"/>
-      <c r="D11" s="188"/>
-      <c r="E11" s="189"/>
+      <c r="B11" s="185"/>
+      <c r="C11" s="185"/>
+      <c r="D11" s="185"/>
+      <c r="E11" s="186"/>
       <c r="F11" s="99"/>
     </row>
     <row r="12" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -12792,13 +12792,13 @@
       <c r="F123" s="99"/>
     </row>
     <row r="124" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A124" s="181" t="s">
+      <c r="A124" s="187" t="s">
         <v>488</v>
       </c>
-      <c r="B124" s="182"/>
-      <c r="C124" s="182"/>
-      <c r="D124" s="182"/>
-      <c r="E124" s="183"/>
+      <c r="B124" s="188"/>
+      <c r="C124" s="188"/>
+      <c r="D124" s="188"/>
+      <c r="E124" s="189"/>
       <c r="F124" s="108" t="s">
         <v>491</v>
       </c>
@@ -14435,19 +14435,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A171:E171"/>
-    <mergeCell ref="A145:E145"/>
-    <mergeCell ref="A147:E147"/>
-    <mergeCell ref="A153:E153"/>
-    <mergeCell ref="A160:E160"/>
-    <mergeCell ref="A164:E164"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="A29:E29"/>
-    <mergeCell ref="A19:E19"/>
     <mergeCell ref="A136:E136"/>
     <mergeCell ref="A118:E118"/>
     <mergeCell ref="A43:E43"/>
@@ -14459,6 +14446,19 @@
     <mergeCell ref="A65:E65"/>
     <mergeCell ref="A124:E124"/>
     <mergeCell ref="A132:E132"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A29:E29"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A171:E171"/>
+    <mergeCell ref="A145:E145"/>
+    <mergeCell ref="A147:E147"/>
+    <mergeCell ref="A153:E153"/>
+    <mergeCell ref="A160:E160"/>
+    <mergeCell ref="A164:E164"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15134,44 +15134,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <SharedWithUsers xmlns="bf601f31-63a1-4825-9216-91d773c5ef9c">
-      <UserInfo>
-        <DisplayName>Erika Osti</DisplayName>
-        <AccountId>534</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Penny Johnson</DisplayName>
-        <AccountId>489</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Ben Childs</DisplayName>
-        <AccountId>643</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Thomas Leeds</DisplayName>
-        <AccountId>459</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Kasmyn Chen</DisplayName>
-        <AccountId>532</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="2799d30d-6731-4efe-ac9b-c4895a8828d9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -15452,23 +15420,50 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <SharedWithUsers xmlns="bf601f31-63a1-4825-9216-91d773c5ef9c">
+      <UserInfo>
+        <DisplayName>Erika Osti</DisplayName>
+        <AccountId>534</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Penny Johnson</DisplayName>
+        <AccountId>489</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Ben Childs</DisplayName>
+        <AccountId>643</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Thomas Leeds</DisplayName>
+        <AccountId>459</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Kasmyn Chen</DisplayName>
+        <AccountId>532</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="2799d30d-6731-4efe-ac9b-c4895a8828d9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="565e1b1d-057e-4d85-b896-01a5881d8a45"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="bf601f31-63a1-4825-9216-91d773c5ef9c"/>
-    <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -15495,9 +15490,14 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="565e1b1d-057e-4d85-b896-01a5881d8a45"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="bf601f31-63a1-4825-9216-91d773c5ef9c"/>
+    <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updates ready for translation.
</commit_message>
<xml_diff>
--- a/app/data/MCCD-localisation-V01.xlsx
+++ b/app/data/MCCD-localisation-V01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JALAT/GIT/medical-certificate-of-cause-of-death/app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3BDC830-AD1D-FC4E-A624-B949FDC350FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB689E3-5750-9443-8D86-2B571DB2F30D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13940" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13940" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Using this document" sheetId="8" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1755" uniqueCount="1182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1755" uniqueCount="1181">
   <si>
     <r>
       <rPr>
@@ -3218,9 +3218,6 @@
   </si>
   <si>
     <t>For example, Ysbyty Athrofaol Cymru (YAC), Caerdydd</t>
-  </si>
-  <si>
-    <t>Find the address using hospital name or postcode</t>
   </si>
   <si>
     <t>Find the address using postcode</t>
@@ -5523,6 +5520,15 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -5539,15 +5545,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6663,13 +6660,13 @@
     </row>
     <row r="10" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A10" s="115" t="s">
+        <v>918</v>
+      </c>
+      <c r="B10" s="115" t="s">
         <v>919</v>
       </c>
-      <c r="B10" s="115" t="s">
+      <c r="C10" s="116" t="s">
         <v>920</v>
-      </c>
-      <c r="C10" s="116" t="s">
-        <v>921</v>
       </c>
       <c r="D10" s="115"/>
       <c r="E10" s="117"/>
@@ -6683,7 +6680,7 @@
         <v>703</v>
       </c>
       <c r="C11" s="116" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="D11" s="115" t="s">
         <v>704</v>
@@ -6699,7 +6696,7 @@
         <v>705</v>
       </c>
       <c r="C12" s="116" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="D12" s="115" t="s">
         <v>706</v>
@@ -6715,7 +6712,7 @@
         <v>707</v>
       </c>
       <c r="C13" s="116" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="D13" s="115" t="s">
         <v>708</v>
@@ -6731,7 +6728,7 @@
         <v>709</v>
       </c>
       <c r="C14" s="116" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="D14" s="115" t="s">
         <v>710</v>
@@ -6785,13 +6782,13 @@
     </row>
     <row r="18" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A18" s="115" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="B18" s="115" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="C18" s="116" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="D18" s="115"/>
       <c r="E18" s="117"/>
@@ -6804,7 +6801,7 @@
         <v>720</v>
       </c>
       <c r="C19" s="116" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="D19" s="115" t="s">
         <v>721</v>
@@ -6979,7 +6976,7 @@
         <v>746</v>
       </c>
       <c r="C31" s="47" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>747</v>
@@ -7037,7 +7034,7 @@
         <v>755</v>
       </c>
       <c r="C35" s="47" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="D35" s="96" t="s">
         <v>651</v>
@@ -7130,7 +7127,7 @@
         <v>772</v>
       </c>
       <c r="C41" s="123" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="D41" s="101" t="s">
         <v>773</v>
@@ -7604,7 +7601,7 @@
         <v>820</v>
       </c>
       <c r="C2" s="129" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D2" s="76" t="s">
         <v>821</v>
@@ -7631,10 +7628,10 @@
         <v>485</v>
       </c>
       <c r="B4" s="157" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="C4" s="136" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D4" s="79" t="s">
         <v>289</v>
@@ -7666,7 +7663,7 @@
         <v>826</v>
       </c>
       <c r="C6" s="136" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D6" s="79" t="s">
         <v>827</v>
@@ -7681,7 +7678,7 @@
         <v>828</v>
       </c>
       <c r="C7" s="136" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="D7" s="157"/>
       <c r="E7" s="133"/>
@@ -7691,10 +7688,10 @@
         <v>485</v>
       </c>
       <c r="B8" s="157" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="C8" s="136" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D8" s="79" t="s">
         <v>289</v>
@@ -7726,7 +7723,7 @@
         <v>829</v>
       </c>
       <c r="C10" s="136" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="D10" s="79" t="s">
         <v>830</v>
@@ -7741,7 +7738,7 @@
         <v>831</v>
       </c>
       <c r="C11" s="136" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="D11" s="157"/>
       <c r="E11" s="133"/>
@@ -7754,7 +7751,7 @@
         <v>832</v>
       </c>
       <c r="C12" s="136" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="D12" s="79" t="s">
         <v>289</v>
@@ -7786,7 +7783,7 @@
         <v>833</v>
       </c>
       <c r="C14" s="136" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="D14" s="79" t="s">
         <v>821</v>
@@ -7801,7 +7798,7 @@
         <v>834</v>
       </c>
       <c r="C15" s="136" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="D15" s="79" t="s">
         <v>835</v>
@@ -7813,10 +7810,10 @@
         <v>485</v>
       </c>
       <c r="B16" s="157" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="C16" s="136" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="D16" s="79" t="s">
         <v>289</v>
@@ -7870,7 +7867,7 @@
     </row>
     <row r="2" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="212" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="B2" s="213"/>
       <c r="C2" s="213"/>
@@ -7897,7 +7894,7 @@
         <v>838</v>
       </c>
       <c r="C4" s="44" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -7919,7 +7916,7 @@
         <v>841</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -7930,7 +7927,7 @@
         <v>842</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -7941,7 +7938,7 @@
         <v>844</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8007,7 +8004,7 @@
         <v>856</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -8052,10 +8049,10 @@
         <v>325</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>1008</v>
+      </c>
+      <c r="C18" s="161" t="s">
         <v>1009</v>
-      </c>
-      <c r="C18" s="161" t="s">
-        <v>1010</v>
       </c>
       <c r="D18" s="162"/>
       <c r="E18" s="30"/>
@@ -8065,17 +8062,17 @@
         <v>325</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C19" s="161" t="s">
         <v>1007</v>
-      </c>
-      <c r="C19" s="161" t="s">
-        <v>1008</v>
       </c>
       <c r="D19" s="162"/>
       <c r="E19" s="30"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="212" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="B20" s="213"/>
       <c r="C20" s="213"/>
@@ -8102,10 +8099,10 @@
         <v>866</v>
       </c>
       <c r="C22" s="44" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -8127,12 +8124,12 @@
         <v>868</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="212" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="B25" s="213"/>
       <c r="C25" s="213"/>
@@ -8145,29 +8142,29 @@
         <v>168</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="160" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="B27" s="4" t="s">
+        <v>1014</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>1015</v>
       </c>
-      <c r="C27" s="5" t="s">
-        <v>1016</v>
-      </c>
       <c r="D27" s="4" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="212" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="B28" s="213"/>
       <c r="C28" s="213"/>
@@ -8180,29 +8177,29 @@
         <v>168</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="144" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>1141</v>
+        <v>1140</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="212" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="B31" s="213"/>
       <c r="C31" s="213"/>
@@ -8215,29 +8212,29 @@
         <v>168</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="192" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>1140</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="212" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="B34" s="213"/>
       <c r="C34" s="213"/>
@@ -8250,29 +8247,29 @@
         <v>168</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>1139</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="212" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="B37" s="213"/>
       <c r="C37" s="213"/>
@@ -8282,18 +8279,18 @@
     </row>
     <row r="38" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="212" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="B39" s="213"/>
       <c r="C39" s="213"/>
@@ -8306,24 +8303,24 @@
         <v>168</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="128" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
     </row>
   </sheetData>
@@ -8387,13 +8384,13 @@
         <v>7</v>
       </c>
       <c r="C2" s="84" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="D2" s="82" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="83" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="F2" s="82"/>
     </row>
@@ -8468,7 +8465,7 @@
     <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>249</v>
@@ -9088,10 +9085,10 @@
     <row r="48" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="70"/>
       <c r="B48" s="141" t="s">
+        <v>936</v>
+      </c>
+      <c r="C48" s="142" t="s">
         <v>937</v>
-      </c>
-      <c r="C48" s="142" t="s">
-        <v>938</v>
       </c>
       <c r="D48" s="70"/>
       <c r="E48" s="143"/>
@@ -9264,21 +9261,21 @@
     <row r="63" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A63" s="70"/>
       <c r="B63" s="141" t="s">
+        <v>939</v>
+      </c>
+      <c r="C63" s="142" t="s">
         <v>940</v>
-      </c>
-      <c r="C63" s="142" t="s">
-        <v>941</v>
       </c>
       <c r="D63" s="70"/>
       <c r="E63" s="143"/>
       <c r="F63" s="144" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="70"/>
       <c r="B64" s="141" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="C64" s="142" t="s">
         <v>863</v>
@@ -9304,32 +9301,32 @@
     </row>
     <row r="67" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B67" s="1" t="s">
+        <v>945</v>
+      </c>
+      <c r="C67" s="2" t="s">
         <v>946</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>947</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B68" s="1" t="s">
+        <v>1042</v>
+      </c>
+      <c r="C68" s="2" t="s">
         <v>1043</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>1044</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B69" s="1" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C69" s="2" t="s">
         <v>1045</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>1046</v>
       </c>
     </row>
     <row r="70" spans="1:3" s="173" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="71" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>103</v>
@@ -9337,146 +9334,146 @@
     </row>
     <row r="72" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
+        <v>1108</v>
+      </c>
+      <c r="C72" s="2" t="s">
         <v>1109</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>1110</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
+        <v>1114</v>
+      </c>
+      <c r="C78" s="2" t="s">
         <v>1115</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>1116</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="80" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
+        <v>1121</v>
+      </c>
+      <c r="C84" s="2" t="s">
         <v>1122</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>1123</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
     </row>
   </sheetData>
@@ -9542,45 +9539,45 @@
     </row>
     <row r="3" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>173</v>
       </c>
       <c r="C3" s="44" t="s">
+        <v>1164</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>1165</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>1166</v>
       </c>
       <c r="E3" s="74"/>
       <c r="F3" s="61"/>
     </row>
     <row r="4" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
+        <v>1157</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>1158</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>1159</v>
-      </c>
       <c r="C4" s="44" t="s">
+        <v>1168</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>1169</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>1170</v>
       </c>
       <c r="E4" s="74"/>
       <c r="F4" s="61"/>
     </row>
     <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="74"/>
@@ -9588,16 +9585,16 @@
     </row>
     <row r="6" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="C6" s="44" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="E6" s="74"/>
       <c r="F6" s="61"/>
@@ -9632,7 +9629,7 @@
         <v>181</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="E8" s="31"/>
       <c r="F8" s="4" t="s">
@@ -9796,10 +9793,10 @@
         <v>168</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>890</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>891</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>892</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="32"/>
@@ -9810,17 +9807,17 @@
         <v>320</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>892</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>893</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>894</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="32"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="178" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="B4" s="179"/>
       <c r="C4" s="179"/>
@@ -9832,10 +9829,10 @@
         <v>168</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="32"/>
@@ -9845,17 +9842,17 @@
         <v>320</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="32"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="178" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="B7" s="179"/>
       <c r="C7" s="179"/>
@@ -9867,36 +9864,36 @@
         <v>168</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>984</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>985</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>986</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="32"/>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
+        <v>986</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>987</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="C9" s="5" t="s">
         <v>988</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>989</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="32"/>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
+        <v>989</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>990</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="C10" s="5" t="s">
         <v>991</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>992</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="32"/>
@@ -9906,10 +9903,10 @@
         <v>168</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="32"/>
@@ -9919,10 +9916,10 @@
         <v>320</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>993</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>994</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>995</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="32"/>
@@ -10054,7 +10051,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="178" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="B2" s="179"/>
       <c r="C2" s="179"/>
@@ -10063,86 +10060,86 @@
     </row>
     <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
+        <v>1047</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>1049</v>
+      </c>
+      <c r="C3" s="163" t="s">
         <v>1048</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>1050</v>
-      </c>
-      <c r="C3" s="163" t="s">
-        <v>1049</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="32"/>
     </row>
     <row r="4" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="C4" s="163" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>1154</v>
+        <v>1153</v>
       </c>
       <c r="E4" s="32"/>
     </row>
     <row r="5" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="C5" s="163" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>1155</v>
+        <v>1154</v>
       </c>
       <c r="E5" s="32"/>
     </row>
     <row r="6" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="C6" s="163" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="E6" s="32"/>
     </row>
     <row r="7" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>1056</v>
+      </c>
+      <c r="C7" s="163" t="s">
         <v>1057</v>
       </c>
-      <c r="C7" s="163" t="s">
-        <v>1058</v>
-      </c>
       <c r="D7" s="4" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="E7" s="32"/>
     </row>
     <row r="8" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>1058</v>
+      </c>
+      <c r="C8" s="163" t="s">
         <v>1059</v>
-      </c>
-      <c r="C8" s="163" t="s">
-        <v>1060</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="32"/>
@@ -10152,23 +10149,23 @@
         <v>168</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="C9" s="163" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="32"/>
     </row>
     <row r="10" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="C10" s="163" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="32"/>
@@ -10178,36 +10175,36 @@
         <v>174</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="C11" s="163" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="32"/>
     </row>
     <row r="12" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="C12" s="163" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="32"/>
     </row>
     <row r="13" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="C13" s="163" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="32"/>
@@ -10217,23 +10214,23 @@
         <v>174</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>1071</v>
+      </c>
+      <c r="C14" s="163" t="s">
         <v>1072</v>
-      </c>
-      <c r="C14" s="163" t="s">
-        <v>1073</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="32"/>
     </row>
     <row r="15" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
+        <v>1073</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>1074</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="C15" s="163" t="s">
         <v>1075</v>
-      </c>
-      <c r="C15" s="163" t="s">
-        <v>1076</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="32"/>
@@ -10243,23 +10240,23 @@
         <v>14</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="C16" s="163" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="32"/>
     </row>
     <row r="17" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="C17" s="163" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="32"/>
@@ -10269,10 +10266,10 @@
         <v>14</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="C18" s="163" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="32"/>
@@ -10282,10 +10279,10 @@
         <v>14</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>1081</v>
+      </c>
+      <c r="C19" s="163" t="s">
         <v>1082</v>
-      </c>
-      <c r="C19" s="163" t="s">
-        <v>1083</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="32"/>
@@ -10323,7 +10320,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{344327F7-D7B0-4B8B-A26A-307F32EA23BD}">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D47" sqref="D47"/>
     </sheetView>
@@ -10380,7 +10377,7 @@
         <v>168</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>188</v>
@@ -10414,10 +10411,10 @@
         <v>192</v>
       </c>
       <c r="C5" s="37" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="D5" s="51" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="E5" s="134"/>
       <c r="F5" s="1" t="s">
@@ -10435,10 +10432,10 @@
         <v>195</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="D6" s="52" t="s">
-        <v>1152</v>
+        <v>1151</v>
       </c>
       <c r="E6" s="135"/>
       <c r="G6" s="52" t="s">
@@ -10453,10 +10450,10 @@
         <v>197</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="D7" s="52" t="s">
-        <v>1153</v>
+        <v>1152</v>
       </c>
       <c r="E7" s="135"/>
       <c r="F7" s="53" t="s">
@@ -10640,7 +10637,7 @@
         <v>236</v>
       </c>
       <c r="C19" s="49" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>237</v>
@@ -10650,10 +10647,10 @@
     <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="6"/>
       <c r="B20" s="6" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="C20" s="174" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="175"/>
@@ -10769,20 +10766,20 @@
     </row>
     <row r="28" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
+        <v>902</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>903</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>904</v>
-      </c>
       <c r="C28" s="5" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="28"/>
     </row>
     <row r="29" spans="1:6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="178" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B29" s="179"/>
       <c r="C29" s="179"/>
@@ -10794,10 +10791,10 @@
         <v>174</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="28"/>
@@ -10807,10 +10804,10 @@
         <v>174</v>
       </c>
       <c r="B31" s="4" t="s">
+        <v>1086</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>1087</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>1088</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="28"/>
@@ -10820,10 +10817,10 @@
         <v>174</v>
       </c>
       <c r="B32" s="4" t="s">
+        <v>1088</v>
+      </c>
+      <c r="C32" s="5" t="s">
         <v>1089</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>1090</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="28"/>
@@ -10833,10 +10830,10 @@
         <v>614</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -10844,21 +10841,21 @@
         <v>14</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -10866,10 +10863,10 @@
         <v>174</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -10877,10 +10874,10 @@
         <v>614</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="16" x14ac:dyDescent="0.2">
@@ -10888,26 +10885,26 @@
         <v>14</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>208</v>
@@ -10915,88 +10912,88 @@
     </row>
     <row r="41" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>1134</v>
+        <v>1133</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>1131</v>
+      </c>
+      <c r="D45" s="1" t="s">
         <v>1134</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>1132</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>1135</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
+        <v>1133</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>1132</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>1134</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>1133</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>1135</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B48" s="1" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="49" spans="2:3" ht="80" x14ac:dyDescent="0.2">
       <c r="B49" s="1" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="50" spans="2:3" ht="16" x14ac:dyDescent="0.2">
       <c r="B50" s="1" t="s">
+        <v>1176</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>1177</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>1178</v>
       </c>
     </row>
   </sheetData>
@@ -11011,9 +11008,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B63483B8-55BE-4CA0-9111-55E5C0AEF6CB}">
   <dimension ref="A1:F291"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A186" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F171" sqref="F171"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A153" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D159" sqref="D159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11048,13 +11045,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="181" t="s">
+      <c r="A2" s="184" t="s">
         <v>259</v>
       </c>
-      <c r="B2" s="182"/>
-      <c r="C2" s="182"/>
-      <c r="D2" s="182"/>
-      <c r="E2" s="183"/>
+      <c r="B2" s="185"/>
+      <c r="C2" s="185"/>
+      <c r="D2" s="185"/>
+      <c r="E2" s="186"/>
       <c r="F2" s="26"/>
     </row>
     <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -11142,10 +11139,10 @@
         <v>271</v>
       </c>
       <c r="B8" s="99" t="s">
+        <v>980</v>
+      </c>
+      <c r="C8" s="97" t="s">
         <v>981</v>
-      </c>
-      <c r="C8" s="97" t="s">
-        <v>982</v>
       </c>
       <c r="D8" s="101"/>
       <c r="E8" s="100"/>
@@ -11182,13 +11179,13 @@
       <c r="F10" s="99"/>
     </row>
     <row r="11" spans="1:6" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="184" t="s">
+      <c r="A11" s="187" t="s">
         <v>282</v>
       </c>
-      <c r="B11" s="185"/>
-      <c r="C11" s="185"/>
-      <c r="D11" s="185"/>
-      <c r="E11" s="186"/>
+      <c r="B11" s="188"/>
+      <c r="C11" s="188"/>
+      <c r="D11" s="188"/>
+      <c r="E11" s="189"/>
       <c r="F11" s="99"/>
     </row>
     <row r="12" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -11299,7 +11296,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="178" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="B19" s="179"/>
       <c r="C19" s="179"/>
@@ -11312,10 +11309,10 @@
         <v>168</v>
       </c>
       <c r="B20" s="111" t="s">
+        <v>961</v>
+      </c>
+      <c r="C20" s="112" t="s">
         <v>962</v>
-      </c>
-      <c r="C20" s="112" t="s">
-        <v>963</v>
       </c>
       <c r="D20" s="94"/>
       <c r="E20" s="110"/>
@@ -11326,13 +11323,13 @@
         <v>267</v>
       </c>
       <c r="B21" s="111" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="C21" s="112" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="D21" s="176" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="E21" s="110"/>
       <c r="F21" s="99"/>
@@ -11342,29 +11339,29 @@
         <v>267</v>
       </c>
       <c r="B22" s="111" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="C22" s="112" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="D22" s="94" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="E22" s="110"/>
       <c r="F22" s="99"/>
     </row>
     <row r="23" spans="1:6" s="156" customFormat="1" ht="80" x14ac:dyDescent="0.2">
       <c r="A23" s="150" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="B23" s="151" t="s">
+        <v>967</v>
+      </c>
+      <c r="C23" s="152" t="s">
         <v>968</v>
       </c>
-      <c r="C23" s="152" t="s">
-        <v>969</v>
-      </c>
       <c r="D23" s="153" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="E23" s="154"/>
       <c r="F23" s="155"/>
@@ -11474,10 +11471,10 @@
         <v>320</v>
       </c>
       <c r="B31" s="96" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="C31" s="44" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="D31" s="96"/>
       <c r="E31" s="100"/>
@@ -11491,10 +11488,10 @@
         <v>321</v>
       </c>
       <c r="C32" s="44" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="D32" s="96" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="E32" s="100"/>
       <c r="F32" s="99"/>
@@ -11603,7 +11600,7 @@
         <v>335</v>
       </c>
       <c r="C40" s="97" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="D40" s="96" t="s">
         <v>336</v>
@@ -11698,10 +11695,10 @@
         <v>320</v>
       </c>
       <c r="B47" s="105" t="s">
+        <v>948</v>
+      </c>
+      <c r="C47" s="145" t="s">
         <v>949</v>
-      </c>
-      <c r="C47" s="145" t="s">
-        <v>950</v>
       </c>
       <c r="D47" s="105"/>
       <c r="E47" s="110"/>
@@ -11811,7 +11808,7 @@
         <v>362</v>
       </c>
       <c r="C54" s="136" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="D54" s="79" t="s">
         <v>289</v>
@@ -11855,7 +11852,7 @@
         <v>367</v>
       </c>
       <c r="C57" s="97" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="D57" s="96"/>
       <c r="E57" s="100"/>
@@ -11953,7 +11950,7 @@
         <v>380</v>
       </c>
       <c r="C64" s="97" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="D64" s="96"/>
       <c r="E64" s="100"/>
@@ -11995,7 +11992,7 @@
         <v>385</v>
       </c>
       <c r="C67" s="97" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="D67" s="96"/>
       <c r="E67" s="100"/>
@@ -12024,7 +12021,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="137" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="C69" s="77" t="s">
         <v>387</v>
@@ -12040,7 +12037,7 @@
         <v>68</v>
       </c>
       <c r="B70" s="137" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="C70" s="77" t="s">
         <v>387</v>
@@ -12056,7 +12053,7 @@
         <v>68</v>
       </c>
       <c r="B71" s="138" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="C71" s="139" t="s">
         <v>387</v>
@@ -12070,7 +12067,7 @@
         <v>68</v>
       </c>
       <c r="B72" s="138" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="C72" s="139" t="s">
         <v>387</v>
@@ -12084,7 +12081,7 @@
         <v>68</v>
       </c>
       <c r="B73" s="138" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="C73" s="139" t="s">
         <v>387</v>
@@ -12435,13 +12432,13 @@
     </row>
     <row r="98" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="96" t="s">
+        <v>950</v>
+      </c>
+      <c r="B98" s="96" t="s">
+        <v>952</v>
+      </c>
+      <c r="C98" s="97" t="s">
         <v>951</v>
-      </c>
-      <c r="B98" s="96" t="s">
-        <v>953</v>
-      </c>
-      <c r="C98" s="97" t="s">
-        <v>952</v>
       </c>
       <c r="D98" s="96"/>
       <c r="E98" s="100"/>
@@ -12449,13 +12446,13 @@
     </row>
     <row r="99" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A99" s="96" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="B99" s="96" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="C99" s="97" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="D99" s="96"/>
       <c r="E99" s="100"/>
@@ -12792,13 +12789,13 @@
       <c r="F123" s="99"/>
     </row>
     <row r="124" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A124" s="187" t="s">
+      <c r="A124" s="181" t="s">
         <v>488</v>
       </c>
-      <c r="B124" s="188"/>
-      <c r="C124" s="188"/>
-      <c r="D124" s="188"/>
-      <c r="E124" s="189"/>
+      <c r="B124" s="182"/>
+      <c r="C124" s="182"/>
+      <c r="D124" s="182"/>
+      <c r="E124" s="183"/>
       <c r="F124" s="108" t="s">
         <v>491</v>
       </c>
@@ -12824,10 +12821,10 @@
         <v>168</v>
       </c>
       <c r="B126" s="96" t="s">
+        <v>996</v>
+      </c>
+      <c r="C126" s="109" t="s">
         <v>997</v>
-      </c>
-      <c r="C126" s="109" t="s">
-        <v>998</v>
       </c>
       <c r="D126" s="94"/>
       <c r="E126" s="110"/>
@@ -12915,7 +12912,7 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" s="178" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="B132" s="179"/>
       <c r="C132" s="179"/>
@@ -12928,10 +12925,10 @@
         <v>168</v>
       </c>
       <c r="B133" s="111" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="C133" s="112" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="D133" s="94"/>
       <c r="E133" s="110"/>
@@ -12939,13 +12936,13 @@
     </row>
     <row r="134" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="B134" s="1" t="s">
+        <v>973</v>
+      </c>
+      <c r="C134" s="2" t="s">
         <v>974</v>
-      </c>
-      <c r="C134" s="2" t="s">
-        <v>975</v>
       </c>
     </row>
     <row r="135" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -12953,13 +12950,13 @@
         <v>179</v>
       </c>
       <c r="B135" s="1" t="s">
+        <v>976</v>
+      </c>
+      <c r="C135" s="2" t="s">
         <v>977</v>
       </c>
-      <c r="C135" s="2" t="s">
-        <v>978</v>
-      </c>
       <c r="D135" s="1" t="s">
-        <v>1149</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.2">
@@ -13012,7 +13009,7 @@
         <v>503</v>
       </c>
       <c r="C139" s="136" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="D139" s="79" t="s">
         <v>289</v>
@@ -13028,7 +13025,7 @@
         <v>504</v>
       </c>
       <c r="C140" s="136" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="D140" s="79" t="s">
         <v>289</v>
@@ -13044,7 +13041,7 @@
         <v>505</v>
       </c>
       <c r="C141" s="136" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="D141" s="79" t="s">
         <v>289</v>
@@ -13086,16 +13083,16 @@
     </row>
     <row r="144" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A144" s="158" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="B144" s="157" t="s">
+        <v>1001</v>
+      </c>
+      <c r="C144" s="159" t="s">
         <v>1002</v>
       </c>
-      <c r="C144" s="159" t="s">
-        <v>1003</v>
-      </c>
       <c r="D144" s="157" t="s">
-        <v>1150</v>
+        <v>1149</v>
       </c>
       <c r="E144" s="133"/>
       <c r="F144" s="99"/>
@@ -13157,10 +13154,10 @@
         <v>320</v>
       </c>
       <c r="B149" s="96" t="s">
+        <v>1003</v>
+      </c>
+      <c r="C149" s="97" t="s">
         <v>1004</v>
-      </c>
-      <c r="C149" s="97" t="s">
-        <v>1005</v>
       </c>
       <c r="D149" s="96"/>
       <c r="E149" s="100"/>
@@ -13274,7 +13271,7 @@
         <v>526</v>
       </c>
       <c r="C157" s="97" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="D157" s="96"/>
       <c r="E157" s="100"/>
@@ -13285,7 +13282,7 @@
         <v>473</v>
       </c>
       <c r="B158" s="96" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="C158" s="97" t="s">
         <v>37</v>
@@ -13299,10 +13296,10 @@
         <v>28</v>
       </c>
       <c r="B159" s="96" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="C159" s="113" t="s">
-        <v>886</v>
+        <v>508</v>
       </c>
       <c r="D159" s="96"/>
       <c r="E159" s="100"/>
@@ -13414,7 +13411,7 @@
         <v>540</v>
       </c>
       <c r="C167" s="97" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="D167" s="96"/>
       <c r="E167" s="100"/>
@@ -13428,7 +13425,7 @@
         <v>541</v>
       </c>
       <c r="C168" s="97" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="D168" s="96"/>
       <c r="E168" s="100"/>
@@ -13442,7 +13439,7 @@
         <v>542</v>
       </c>
       <c r="C169" s="97" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="D169" s="96"/>
       <c r="E169" s="100"/>
@@ -13512,7 +13509,7 @@
         <v>551</v>
       </c>
       <c r="C174" s="44" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="D174" s="96" t="s">
         <v>552</v>
@@ -14435,6 +14432,19 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A171:E171"/>
+    <mergeCell ref="A145:E145"/>
+    <mergeCell ref="A147:E147"/>
+    <mergeCell ref="A153:E153"/>
+    <mergeCell ref="A160:E160"/>
+    <mergeCell ref="A164:E164"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A11:E11"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A29:E29"/>
+    <mergeCell ref="A19:E19"/>
     <mergeCell ref="A136:E136"/>
     <mergeCell ref="A118:E118"/>
     <mergeCell ref="A43:E43"/>
@@ -14446,19 +14456,6 @@
     <mergeCell ref="A65:E65"/>
     <mergeCell ref="A124:E124"/>
     <mergeCell ref="A132:E132"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A11:E11"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="A29:E29"/>
-    <mergeCell ref="A19:E19"/>
-    <mergeCell ref="A171:E171"/>
-    <mergeCell ref="A145:E145"/>
-    <mergeCell ref="A147:E147"/>
-    <mergeCell ref="A153:E153"/>
-    <mergeCell ref="A160:E160"/>
-    <mergeCell ref="A164:E164"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14571,10 +14568,10 @@
     </row>
     <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B8" s="146" t="s">
+        <v>958</v>
+      </c>
+      <c r="C8" s="147" t="s">
         <v>959</v>
-      </c>
-      <c r="C8" s="147" t="s">
-        <v>960</v>
       </c>
       <c r="D8" s="146"/>
       <c r="E8" s="148"/>
@@ -14751,7 +14748,7 @@
         <v>618</v>
       </c>
       <c r="C22" s="66" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="D22" s="64"/>
       <c r="E22" s="65"/>
@@ -14851,7 +14848,7 @@
         <v>635</v>
       </c>
       <c r="D30" s="157" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="E30" s="73"/>
     </row>
@@ -14863,7 +14860,7 @@
         <v>636</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -14871,10 +14868,10 @@
         <v>179</v>
       </c>
       <c r="B32" s="16" t="s">
+        <v>910</v>
+      </c>
+      <c r="C32" s="18" t="s">
         <v>911</v>
-      </c>
-      <c r="C32" s="18" t="s">
-        <v>912</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -14962,7 +14959,7 @@
         <v>650</v>
       </c>
       <c r="C39" s="47" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="D39" s="96" t="s">
         <v>651</v>
@@ -15143,6 +15140,47 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <SharedWithUsers xmlns="bf601f31-63a1-4825-9216-91d773c5ef9c">
+      <UserInfo>
+        <DisplayName>Erika Osti</DisplayName>
+        <AccountId>534</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Penny Johnson</DisplayName>
+        <AccountId>489</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Ben Childs</DisplayName>
+        <AccountId>643</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Thomas Leeds</DisplayName>
+        <AccountId>459</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Kasmyn Chen</DisplayName>
+        <AccountId>532</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="2799d30d-6731-4efe-ac9b-c4895a8828d9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010096D84A54A9CD274097F17166F184737D" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2fd95a4cfdf4f2f51219070f5dff16a8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="565e1b1d-057e-4d85-b896-01a5881d8a45" xmlns:ns3="bf601f31-63a1-4825-9216-91d773c5ef9c" xmlns:ns4="2799d30d-6731-4efe-ac9b-c4895a8828d9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f7499f6f4dc8ad2a533df04863f63fa7" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -15419,47 +15457,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Readyforteam_x003f_ xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">false</Readyforteam_x003f_>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <SharedWithUsers xmlns="bf601f31-63a1-4825-9216-91d773c5ef9c">
-      <UserInfo>
-        <DisplayName>Erika Osti</DisplayName>
-        <AccountId>534</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Penny Johnson</DisplayName>
-        <AccountId>489</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Ben Childs</DisplayName>
-        <AccountId>643</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Thomas Leeds</DisplayName>
-        <AccountId>459</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Kasmyn Chen</DisplayName>
-        <AccountId>532</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="565e1b1d-057e-4d85-b896-01a5881d8a45">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="2799d30d-6731-4efe-ac9b-c4895a8828d9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D7CE8C7-18DC-484F-8376-ED09F13D44C8}">
   <ds:schemaRefs>
@@ -15469,6 +15466,19 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="565e1b1d-057e-4d85-b896-01a5881d8a45"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="bf601f31-63a1-4825-9216-91d773c5ef9c"/>
+    <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EAFDB110-4046-4E72-A1EF-1908ABEC3151}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15487,17 +15497,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{017ACE96-8143-486E-8436-7787F6B96F4A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="565e1b1d-057e-4d85-b896-01a5881d8a45"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="bf601f31-63a1-4825-9216-91d773c5ef9c"/>
-    <ds:schemaRef ds:uri="2799d30d-6731-4efe-ac9b-c4895a8828d9"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>